<commit_message>
Run more clustering for finding k
</commit_message>
<xml_diff>
--- a/Documentation/Plots.xlsx
+++ b/Documentation/Plots.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/MSE/Cours/MA_BDA/Projet/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB0090B-98EC-E94E-AC38-53886450BB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745AE028-F1E5-3843-90A8-21418AC20D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" activeTab="2" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="clusteringScore0" sheetId="1" r:id="rId1"/>
-    <sheet name="clusteringScore1" sheetId="3" r:id="rId2"/>
+    <sheet name="clusteringScore0 (20-300)" sheetId="1" r:id="rId1"/>
+    <sheet name="clusteringScore1 (20-300)" sheetId="3" r:id="rId2"/>
+    <sheet name="clusteringScore0 (200-280)" sheetId="4" r:id="rId3"/>
+    <sheet name="clusteringScore1 (200-280)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>K</t>
   </si>
@@ -48,6 +50,12 @@
   </si>
   <si>
     <t>clusteringScore1</t>
+  </si>
+  <si>
+    <t>First run</t>
+  </si>
+  <si>
+    <t>Second run</t>
   </si>
 </sst>
 </file>
@@ -278,50 +286,28 @@
     <xf numFmtId="11" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
         <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9"/>
       </font>
       <fill>
         <patternFill>
@@ -343,11 +329,85 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -438,7 +498,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>clusteringScore0!$D$4</c:f>
+              <c:f>'clusteringScore0 (20-300)'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -512,7 +572,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>clusteringScore0!$C$5:$C$33</c:f>
+              <c:f>'clusteringScore0 (20-300)'!$C$5:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -608,7 +668,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>clusteringScore0!$D$5:$D$33</c:f>
+              <c:f>'clusteringScore0 (20-300)'!$D$5:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="29"/>
@@ -1030,7 +1090,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>clusteringScore1!$D$4</c:f>
+              <c:f>'clusteringScore1 (20-300)'!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1104,7 +1164,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>clusteringScore1!$C$5:$C$33</c:f>
+              <c:f>'clusteringScore1 (20-300)'!$C$5:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -1200,7 +1260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>clusteringScore1!$D$5:$D$33</c:f>
+              <c:f>'clusteringScore1 (20-300)'!$D$5:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="29"/>
@@ -1548,6 +1608,1460 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>clusteringScore0</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore0 (200-280)'!$C$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>First run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore0 (200-280)'!$C$5:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore0 (200-280)'!$D$5:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>43115686606281.398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37520679370712.703</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38640547308276.102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71715343203501.406</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31744015039013.801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34957344793768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16584203609327.801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10538508016393.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10768915085790.699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17181743716637</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27641759026384.801</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45391078362974.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36078974902365.898</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12350053202754.801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12862964277883.699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26530470181834.801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6842574109661.5703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A9AA-2D4A-A8F9-F5694B13ED6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore0 (200-280)'!$F$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Second run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore0 (200-280)'!$F$5:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore0 (200-280)'!$G$5:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>21874556623540.699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35430352759950.203</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15369723939769.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27982663175584.199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24299106101254.102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21780231441946.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22062024343069.199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45309356678723.398</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8772768516759.3301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13145553681154.699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9152575417728.3809</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19188330194304.301</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38633875983042.797</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8080824746270.3604</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33106354028649.699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18068595945199</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7283842868399.3701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A9AA-2D4A-A8F9-F5694B13ED6E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1510166927"/>
+        <c:axId val="1510168575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1510166927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="280"/>
+          <c:min val="195"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510168575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1510168575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510166927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>clusteringScore1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore1 (200-280)'!$C$3:$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>First run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore1 (200-280)'!$C$5:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore1 (200-280)'!$D$5:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>21778254123155.398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24506902426529.602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10835109567610.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9906278158060.1602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7952564528623.0498</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15948729483872.199</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7569436700428.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31660211694151.102</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24170329822640.398</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38181093826685</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15992280437112</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20214978498802.898</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47964968188028.398</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21394877672669.102</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13641212881476.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>42135170942794.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17254612097701.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E911-8943-9D78-67075DD9ED80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore1 (200-280)'!$F$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Second run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore1 (200-280)'!$F$5:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>280</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore1 (200-280)'!$G$5:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>52066707397160.703</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12625333169428.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17997338026058.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35686209667907.797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3983436481834.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8708526170976.9004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22714461452789.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9209183972625.5508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40222189806689.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14481145516512.301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13655548087417.801</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19441129998611.102</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26715018373696.102</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12753995295845.801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8007479812460.5996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9669702811797.4297</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16010048607154.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E911-8943-9D78-67075DD9ED80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1510166927"/>
+        <c:axId val="1510168575"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1510166927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="280"/>
+          <c:min val="195"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>k</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510168575"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+        <c:minorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1510168575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-CH"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1510166927"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
@@ -1622,6 +3136,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
@@ -2102,6 +3690,964 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2642,6 +5188,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99D83CC8-C643-4E40-B2AF-0BB4609EF01F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{555BE799-6EB3-D34B-8D84-D9215705E5DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFBB0168-E59F-764B-A9BE-05E466FC53CD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2996,10 +5628,10 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3016,10 +5648,10 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
@@ -3697,7 +6329,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3710,8 +6342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1735262A-9A28-5748-B32C-17C88F0166F4}">
   <dimension ref="B1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3743,10 +6375,10 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -3763,10 +6395,10 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
@@ -4444,11 +7076,1813 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC794971-B799-6141-9B75-3FE637FEF510}">
+  <dimension ref="B1:T34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" customWidth="1"/>
+    <col min="20" max="20" width="2.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="11">
+        <v>200</v>
+      </c>
+      <c r="D5" s="12">
+        <v>43115686606281.398</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="11">
+        <v>200</v>
+      </c>
+      <c r="G5" s="12">
+        <v>21874556623540.699</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="11">
+        <v>205</v>
+      </c>
+      <c r="D6" s="12">
+        <v>37520679370712.703</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="11">
+        <v>205</v>
+      </c>
+      <c r="G6" s="12">
+        <v>35430352759950.203</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="11">
+        <v>210</v>
+      </c>
+      <c r="D7" s="12">
+        <v>38640547308276.102</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="11">
+        <v>210</v>
+      </c>
+      <c r="G7" s="12">
+        <v>15369723939769.1</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="11">
+        <v>215</v>
+      </c>
+      <c r="D8" s="12">
+        <v>71715343203501.406</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="11">
+        <v>215</v>
+      </c>
+      <c r="G8" s="12">
+        <v>27982663175584.199</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="11">
+        <v>220</v>
+      </c>
+      <c r="D9" s="12">
+        <v>31744015039013.801</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="11">
+        <v>220</v>
+      </c>
+      <c r="G9" s="12">
+        <v>24299106101254.102</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="11">
+        <v>225</v>
+      </c>
+      <c r="D10" s="12">
+        <v>34957344793768</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="11">
+        <v>225</v>
+      </c>
+      <c r="G10" s="12">
+        <v>21780231441946.5</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="11">
+        <v>230</v>
+      </c>
+      <c r="D11" s="12">
+        <v>16584203609327.801</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="11">
+        <v>230</v>
+      </c>
+      <c r="G11" s="12">
+        <v>22062024343069.199</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="11">
+        <v>235</v>
+      </c>
+      <c r="D12" s="12">
+        <v>10538508016393.5</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="11">
+        <v>235</v>
+      </c>
+      <c r="G12" s="12">
+        <v>45309356678723.398</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="11">
+        <v>240</v>
+      </c>
+      <c r="D13" s="12">
+        <v>10768915085790.699</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11">
+        <v>240</v>
+      </c>
+      <c r="G13" s="12">
+        <v>8772768516759.3301</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="11">
+        <v>245</v>
+      </c>
+      <c r="D14" s="12">
+        <v>17181743716637</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="11">
+        <v>245</v>
+      </c>
+      <c r="G14" s="12">
+        <v>13145553681154.699</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="11">
+        <v>250</v>
+      </c>
+      <c r="D15" s="12">
+        <v>27641759026384.801</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11">
+        <v>250</v>
+      </c>
+      <c r="G15" s="12">
+        <v>9152575417728.3809</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="11">
+        <v>255</v>
+      </c>
+      <c r="D16" s="12">
+        <v>45391078362974.5</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11">
+        <v>255</v>
+      </c>
+      <c r="G16" s="12">
+        <v>19188330194304.301</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="11">
+        <v>260</v>
+      </c>
+      <c r="D17" s="12">
+        <v>36078974902365.898</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="11">
+        <v>260</v>
+      </c>
+      <c r="G17" s="12">
+        <v>38633875983042.797</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="11">
+        <v>265</v>
+      </c>
+      <c r="D18" s="12">
+        <v>12350053202754.801</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="11">
+        <v>265</v>
+      </c>
+      <c r="G18" s="12">
+        <v>8080824746270.3604</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="11">
+        <v>270</v>
+      </c>
+      <c r="D19" s="12">
+        <v>12862964277883.699</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="11">
+        <v>270</v>
+      </c>
+      <c r="G19" s="12">
+        <v>33106354028649.699</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="11">
+        <v>275</v>
+      </c>
+      <c r="D20" s="12">
+        <v>26530470181834.801</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="11">
+        <v>275</v>
+      </c>
+      <c r="G20" s="12">
+        <v>18068595945199</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="11">
+        <v>280</v>
+      </c>
+      <c r="D21" s="12">
+        <v>6842574109661.5703</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="11">
+        <v>280</v>
+      </c>
+      <c r="G21" s="12">
+        <v>7283842868399.3701</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="11">
+        <v>285</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="11">
+        <v>285</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="11">
+        <v>290</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="11">
+        <v>290</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="11">
+        <v>295</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="11">
+        <v>295</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="6"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="11">
+        <v>300</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="11">
+        <v>300</v>
+      </c>
+      <c r="G25" s="12"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="11">
+        <v>305</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="11">
+        <v>305</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="6"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="11">
+        <v>310</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="11">
+        <v>310</v>
+      </c>
+      <c r="G27" s="12"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="11">
+        <v>315</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="11">
+        <v>315</v>
+      </c>
+      <c r="G28" s="12"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="11">
+        <v>320</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="11">
+        <v>320</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="6"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5:D33">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>D5=MIN($D$5:$D$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G33">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>G22=MIN($D$5:$D$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G21">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>G5=MIN($G$5:$G$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10CBAC2-FB0E-0146-80D2-7AAE88CD07D0}">
+  <dimension ref="B1:T34"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" customWidth="1"/>
+    <col min="20" max="20" width="2.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="11">
+        <v>200</v>
+      </c>
+      <c r="D5" s="12">
+        <v>21778254123155.398</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="11">
+        <v>200</v>
+      </c>
+      <c r="G5" s="12">
+        <v>52066707397160.703</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="11">
+        <v>205</v>
+      </c>
+      <c r="D6" s="12">
+        <v>24506902426529.602</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="11">
+        <v>205</v>
+      </c>
+      <c r="G6" s="12">
+        <v>12625333169428.5</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="11">
+        <v>210</v>
+      </c>
+      <c r="D7" s="12">
+        <v>10835109567610.5</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="11">
+        <v>210</v>
+      </c>
+      <c r="G7" s="12">
+        <v>17997338026058.5</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="11">
+        <v>215</v>
+      </c>
+      <c r="D8" s="12">
+        <v>9906278158060.1602</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="11">
+        <v>215</v>
+      </c>
+      <c r="G8" s="12">
+        <v>35686209667907.797</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="5"/>
+      <c r="C9" s="11">
+        <v>220</v>
+      </c>
+      <c r="D9" s="12">
+        <v>7952564528623.0498</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="11">
+        <v>220</v>
+      </c>
+      <c r="G9" s="12">
+        <v>3983436481834.5</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="5"/>
+      <c r="C10" s="11">
+        <v>225</v>
+      </c>
+      <c r="D10" s="12">
+        <v>15948729483872.199</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="11">
+        <v>225</v>
+      </c>
+      <c r="G10" s="12">
+        <v>8708526170976.9004</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="11">
+        <v>230</v>
+      </c>
+      <c r="D11" s="12">
+        <v>7569436700428.54</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="11">
+        <v>230</v>
+      </c>
+      <c r="G11" s="12">
+        <v>22714461452789.5</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="11">
+        <v>235</v>
+      </c>
+      <c r="D12" s="12">
+        <v>31660211694151.102</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="11">
+        <v>235</v>
+      </c>
+      <c r="G12" s="12">
+        <v>9209183972625.5508</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="11">
+        <v>240</v>
+      </c>
+      <c r="D13" s="12">
+        <v>24170329822640.398</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11">
+        <v>240</v>
+      </c>
+      <c r="G13" s="12">
+        <v>40222189806689.5</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="C14" s="11">
+        <v>245</v>
+      </c>
+      <c r="D14" s="12">
+        <v>38181093826685</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="11">
+        <v>245</v>
+      </c>
+      <c r="G14" s="12">
+        <v>14481145516512.301</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="5"/>
+      <c r="C15" s="11">
+        <v>250</v>
+      </c>
+      <c r="D15" s="12">
+        <v>15992280437112</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="11">
+        <v>250</v>
+      </c>
+      <c r="G15" s="12">
+        <v>13655548087417.801</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="C16" s="11">
+        <v>255</v>
+      </c>
+      <c r="D16" s="12">
+        <v>20214978498802.898</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11">
+        <v>255</v>
+      </c>
+      <c r="G16" s="12">
+        <v>19441129998611.102</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="C17" s="11">
+        <v>260</v>
+      </c>
+      <c r="D17" s="12">
+        <v>47964968188028.398</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="11">
+        <v>260</v>
+      </c>
+      <c r="G17" s="12">
+        <v>26715018373696.102</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="11">
+        <v>265</v>
+      </c>
+      <c r="D18" s="12">
+        <v>21394877672669.102</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="11">
+        <v>265</v>
+      </c>
+      <c r="G18" s="12">
+        <v>12753995295845.801</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="11">
+        <v>270</v>
+      </c>
+      <c r="D19" s="12">
+        <v>13641212881476.9</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="11">
+        <v>270</v>
+      </c>
+      <c r="G19" s="12">
+        <v>8007479812460.5996</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="11">
+        <v>275</v>
+      </c>
+      <c r="D20" s="12">
+        <v>42135170942794.5</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="11">
+        <v>275</v>
+      </c>
+      <c r="G20" s="12">
+        <v>9669702811797.4297</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="C21" s="11">
+        <v>280</v>
+      </c>
+      <c r="D21" s="12">
+        <v>17254612097701.5</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="11">
+        <v>280</v>
+      </c>
+      <c r="G21" s="12">
+        <v>16010048607154.1</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="6"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="6"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="6"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5:D33">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>D5=MIN($D$5:$D$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22:G33">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>G22=MIN($D$5:$D$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G21">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>G5=MIN($G$5:$G$33)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New run on clusteringScore3
</commit_message>
<xml_diff>
--- a/Documentation/Plots.xlsx
+++ b/Documentation/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/MSE/Cours/MA_BDA/Projet/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0793F46D-07D6-6B4C-923B-911367471F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AA1726-3D77-9C48-9B23-3D97C838B50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" firstSheet="10" activeTab="16" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" firstSheet="9" activeTab="9" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
   </bookViews>
   <sheets>
     <sheet name="clusteringScore0 (20-300)" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="12">
   <si>
     <t>K</t>
   </si>
@@ -85,6 +85,9 @@
   <si>
     <t>clusteringScore7</t>
   </si>
+  <si>
+    <t>Third run</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +142,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -400,11 +409,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -458,6 +493,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2791,6 +2832,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
                 <c:pt idx="8">
                   <c:v>140</c:v>
                 </c:pt>
@@ -2841,6 +2906,18 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2851,8 +2928,32 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>38322687.631342202</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34063974.356206901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25571685.092843201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22449998.473370701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16323799.488330601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14909185.8359142</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14942180.884695999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12444971.595679</c:v>
+                </c:pt>
                 <c:pt idx="8">
-                  <c:v>11947841.6500184</c:v>
+                  <c:v>12606598.2710234</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10568364.8614564</c:v>
@@ -2900,7 +3001,19 @@
                   <c:v>6888752.8709281404</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5889397.2323465999</c:v>
+                  <c:v>6058938.7756981598</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5777053.1980853099</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5396898.85937637</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5680810.4093086598</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5771874.8301354004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5232,6 +5345,85 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-109B-4E44-8E86-77344693C633}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore4 (160-200)'!$I$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Third run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore4 (160-200)'!$I$5:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore4 (160-200)'!$J$5:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="41"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5247-9247-A767-107483780A5A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23900,13 +24092,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -25541,8 +25733,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="B1:Z34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25583,7 +25775,12 @@
       <c r="W2" s="17">
         <v>51176142.427075498</v>
       </c>
-      <c r="Z2" s="17"/>
+      <c r="Y2">
+        <v>100</v>
+      </c>
+      <c r="Z2" s="17">
+        <v>38322687.631342202</v>
+      </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="5"/>
@@ -25615,7 +25812,12 @@
       <c r="W3" s="17">
         <v>35486889.788498498</v>
       </c>
-      <c r="Z3" s="17"/>
+      <c r="Y3">
+        <v>105</v>
+      </c>
+      <c r="Z3" s="17">
+        <v>34063974.356206901</v>
+      </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B4" s="5"/>
@@ -25651,7 +25853,12 @@
       <c r="W4" s="17">
         <v>27575213.0424302</v>
       </c>
-      <c r="Z4" s="17"/>
+      <c r="Y4">
+        <v>110</v>
+      </c>
+      <c r="Z4" s="17">
+        <v>25571685.092843201</v>
+      </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B5" s="5"/>
@@ -25662,8 +25869,12 @@
         <v>51176142.427075498</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
+      <c r="F5" s="11">
+        <v>100</v>
+      </c>
+      <c r="G5" s="12">
+        <v>38322687.631342202</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -25683,7 +25894,12 @@
       <c r="W5" s="17">
         <v>21946481.744105399</v>
       </c>
-      <c r="Z5" s="17"/>
+      <c r="Y5">
+        <v>115</v>
+      </c>
+      <c r="Z5" s="17">
+        <v>22449998.473370701</v>
+      </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
@@ -25694,8 +25910,12 @@
         <v>35486889.788498498</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="F6" s="11">
+        <v>105</v>
+      </c>
+      <c r="G6" s="12">
+        <v>34063974.356206901</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -25715,7 +25935,12 @@
       <c r="W6" s="17">
         <v>15648145.102177599</v>
       </c>
-      <c r="Z6" s="17"/>
+      <c r="Y6">
+        <v>120</v>
+      </c>
+      <c r="Z6" s="17">
+        <v>16323799.488330601</v>
+      </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
@@ -25726,8 +25951,12 @@
         <v>27575213.0424302</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="F7" s="11">
+        <v>110</v>
+      </c>
+      <c r="G7" s="12">
+        <v>25571685.092843201</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -25747,6 +25976,12 @@
       <c r="W7" s="17">
         <v>15814901.158835201</v>
       </c>
+      <c r="Y7">
+        <v>125</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>14909185.8359142</v>
+      </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
@@ -25757,8 +25992,12 @@
         <v>21946481.744105399</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="11">
+        <v>115</v>
+      </c>
+      <c r="G8" s="12">
+        <v>22449998.473370701</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -25778,6 +26017,12 @@
       <c r="W8" s="17">
         <v>13593415.591743501</v>
       </c>
+      <c r="Y8">
+        <v>130</v>
+      </c>
+      <c r="Z8" s="17">
+        <v>14942180.884695999</v>
+      </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
@@ -25788,8 +26033,12 @@
         <v>15648145.102177599</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="F9" s="11">
+        <v>120</v>
+      </c>
+      <c r="G9" s="12">
+        <v>16323799.488330601</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -25809,6 +26058,12 @@
       <c r="W9" s="17">
         <v>12648191.963459</v>
       </c>
+      <c r="Y9">
+        <v>135</v>
+      </c>
+      <c r="Z9" s="17">
+        <v>12444971.595679</v>
+      </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
@@ -25819,8 +26074,12 @@
         <v>15814901.158835201</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="F10" s="11">
+        <v>125</v>
+      </c>
+      <c r="G10" s="12">
+        <v>14909185.8359142</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -25840,6 +26099,12 @@
       <c r="W10" s="17">
         <v>12038612.1072968</v>
       </c>
+      <c r="Y10">
+        <v>140</v>
+      </c>
+      <c r="Z10" s="17">
+        <v>12606598.2710234</v>
+      </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
@@ -25850,8 +26115,12 @@
         <v>13593415.591743501</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="F11" s="11">
+        <v>130</v>
+      </c>
+      <c r="G11" s="12">
+        <v>14942180.884695999</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -25881,8 +26150,12 @@
         <v>12648191.963459</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
+      <c r="F12" s="11">
+        <v>135</v>
+      </c>
+      <c r="G12" s="12">
+        <v>12444971.595679</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -25916,7 +26189,7 @@
         <v>140</v>
       </c>
       <c r="G13" s="12">
-        <v>11947841.6500184</v>
+        <v>12606598.2710234</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -26043,7 +26316,7 @@
         <v>9532279.1820793208</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
       <c r="C17" s="11">
         <v>160</v>
@@ -26078,7 +26351,7 @@
         <v>8798253.2418077905</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
       <c r="C18" s="11">
         <v>165</v>
@@ -26113,7 +26386,7 @@
         <v>8141894.7778033698</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="11">
         <v>170</v>
@@ -26148,7 +26421,7 @@
         <v>7272787.1134756301</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="11">
         <v>175</v>
@@ -26183,7 +26456,7 @@
         <v>7577602.5882262299</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="5"/>
       <c r="C21" s="11">
         <v>180</v>
@@ -26218,7 +26491,7 @@
         <v>7134927.8113899101</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="11">
         <v>185</v>
@@ -26253,7 +26526,7 @@
         <v>6814834.6363244103</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
       <c r="C23" s="11">
         <v>190</v>
@@ -26288,7 +26561,7 @@
         <v>6387348.8563740198</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
       <c r="C24" s="11">
         <v>195</v>
@@ -26323,7 +26596,7 @@
         <v>6015364.7425185703</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="11">
         <v>200</v>
@@ -26358,7 +26631,7 @@
         <v>6524965.26148214</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="11">
         <v>205</v>
@@ -26392,8 +26665,14 @@
       <c r="W26">
         <v>5862782.8079099404</v>
       </c>
-    </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y26">
+        <v>220</v>
+      </c>
+      <c r="Z26">
+        <v>6058938.7756981598</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="11">
         <v>210</v>
@@ -26427,8 +26706,14 @@
       <c r="W27">
         <v>6117034.9567857999</v>
       </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y27">
+        <v>225</v>
+      </c>
+      <c r="Z27">
+        <v>5777053.1980853099</v>
+      </c>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="11">
         <v>215</v>
@@ -26462,8 +26747,14 @@
       <c r="W28">
         <v>5845145.4594156696</v>
       </c>
-    </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y28">
+        <v>230</v>
+      </c>
+      <c r="Z28">
+        <v>5396898.85937637</v>
+      </c>
+    </row>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
       <c r="C29" s="11">
         <v>220</v>
@@ -26476,7 +26767,7 @@
         <v>220</v>
       </c>
       <c r="G29" s="12">
-        <v>5889397.2323465999</v>
+        <v>6058938.7756981598</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -26497,8 +26788,14 @@
       <c r="W29">
         <v>5440440.6761791399</v>
       </c>
-    </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y29">
+        <v>235</v>
+      </c>
+      <c r="Z29">
+        <v>5680810.4093086598</v>
+      </c>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="11">
         <v>225</v>
@@ -26507,8 +26804,12 @@
         <v>6117034.9567857999</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="12"/>
+      <c r="F30" s="11">
+        <v>225</v>
+      </c>
+      <c r="G30" s="12">
+        <v>5777053.1980853099</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -26528,8 +26829,14 @@
       <c r="W30">
         <v>5443475.0496180998</v>
       </c>
-    </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y30">
+        <v>240</v>
+      </c>
+      <c r="Z30">
+        <v>5771874.8301354004</v>
+      </c>
+    </row>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
       <c r="C31" s="11">
         <v>230</v>
@@ -26538,8 +26845,12 @@
         <v>5845145.4594156696</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="12"/>
+      <c r="F31" s="11">
+        <v>230</v>
+      </c>
+      <c r="G31" s="12">
+        <v>5396898.85937637</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -26560,7 +26871,7 @@
         <v>6073878.9605730204</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B32" s="5"/>
       <c r="C32" s="11">
         <v>235</v>
@@ -26569,8 +26880,12 @@
         <v>5440440.6761791399</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="12"/>
+      <c r="F32" s="11">
+        <v>235</v>
+      </c>
+      <c r="G32" s="12">
+        <v>5680810.4093086598</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -26600,8 +26915,12 @@
         <v>5443475.0496180998</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
+      <c r="F33" s="13">
+        <v>240</v>
+      </c>
+      <c r="G33" s="14">
+        <v>5771874.8301354004</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -26678,7 +26997,7 @@
   <dimension ref="B1:Q34"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28337,25 +28656,30 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523A12C9-FA7D-7048-AB9D-085DF741B38F}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="B1:Z46"/>
+  <dimension ref="B1:AC46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X49" sqref="X49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD31" sqref="AD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="2.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="2.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="2.83203125" customWidth="1"/>
-    <col min="20" max="20" width="2.83203125" customWidth="1"/>
-    <col min="24" max="24" width="4" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" customWidth="1"/>
+    <col min="23" max="23" width="2.83203125" customWidth="1"/>
+    <col min="27" max="27" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -28374,21 +28698,24 @@
       <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
       <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
-      <c r="V2">
-        <v>160</v>
-      </c>
-      <c r="W2" s="17">
-        <v>1.8548850592633202E-2</v>
-      </c>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="20"/>
       <c r="Y2">
         <v>160</v>
       </c>
       <c r="Z2" s="17">
+        <v>1.8548850592633202E-2</v>
+      </c>
+      <c r="AB2">
+        <v>160</v>
+      </c>
+      <c r="AC2" s="17">
         <v>1.73156928908479E-2</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
       <c r="C3" s="27" t="s">
         <v>4</v>
@@ -28400,8 +28727,10 @@
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -28411,21 +28740,24 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="22"/>
-      <c r="V3">
-        <v>161</v>
-      </c>
-      <c r="W3" s="17">
-        <v>2.0957961831983899E-2</v>
-      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="22"/>
       <c r="Y3">
         <v>161</v>
       </c>
       <c r="Z3" s="17">
+        <v>2.0957961831983899E-2</v>
+      </c>
+      <c r="AB3">
+        <v>161</v>
+      </c>
+      <c r="AC3" s="17">
         <v>1.8384753218102901E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B4" s="21"/>
       <c r="C4" s="15" t="s">
         <v>0</v>
@@ -28441,8 +28773,12 @@
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>1</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -28452,21 +28788,24 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="22"/>
-      <c r="V4">
-        <v>162</v>
-      </c>
-      <c r="W4" s="17">
-        <v>1.37115952998703E-2</v>
-      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="22"/>
       <c r="Y4">
         <v>162</v>
       </c>
       <c r="Z4" s="17">
+        <v>1.37115952998703E-2</v>
+      </c>
+      <c r="AB4">
+        <v>162</v>
+      </c>
+      <c r="AC4" s="17">
         <v>1.3799234120787599E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
       <c r="C5" s="11">
         <v>160</v>
@@ -28482,8 +28821,8 @@
         <v>1.73156928908479E-2</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -28493,21 +28832,24 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="22"/>
-      <c r="V5">
-        <v>163</v>
-      </c>
-      <c r="W5" s="17">
-        <v>1.4286521512344901E-2</v>
-      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="22"/>
       <c r="Y5">
         <v>163</v>
       </c>
       <c r="Z5" s="17">
+        <v>1.4286521512344901E-2</v>
+      </c>
+      <c r="AB5">
+        <v>163</v>
+      </c>
+      <c r="AC5" s="17">
         <v>1.3864895400583801E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B6" s="21"/>
       <c r="C6" s="11">
         <v>161</v>
@@ -28523,8 +28865,8 @@
         <v>1.8384753218102901E-2</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -28534,21 +28876,24 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="22"/>
-      <c r="V6">
-        <v>164</v>
-      </c>
-      <c r="W6">
-        <v>1.91952196167876E-2</v>
-      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="22"/>
       <c r="Y6">
         <v>164</v>
       </c>
       <c r="Z6">
+        <v>1.91952196167876E-2</v>
+      </c>
+      <c r="AB6">
+        <v>164</v>
+      </c>
+      <c r="AC6">
         <v>1.2291530168351701E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
       <c r="C7" s="11">
         <v>162</v>
@@ -28564,8 +28909,8 @@
         <v>1.3799234120787599E-2</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -28575,21 +28920,24 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="22"/>
-      <c r="V7">
-        <v>165</v>
-      </c>
-      <c r="W7">
-        <v>1.77636064276235E-2</v>
-      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="22"/>
       <c r="Y7">
         <v>165</v>
       </c>
       <c r="Z7">
+        <v>1.77636064276235E-2</v>
+      </c>
+      <c r="AB7">
+        <v>165</v>
+      </c>
+      <c r="AC7">
         <v>1.7212899751081399E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B8" s="21"/>
       <c r="C8" s="11">
         <v>163</v>
@@ -28605,8 +28953,8 @@
         <v>1.3864895400583801E-2</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -28616,21 +28964,24 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="22"/>
-      <c r="V8">
-        <v>166</v>
-      </c>
-      <c r="W8">
-        <v>1.82826836453591E-2</v>
-      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="22"/>
       <c r="Y8">
         <v>166</v>
       </c>
       <c r="Z8">
+        <v>1.82826836453591E-2</v>
+      </c>
+      <c r="AB8">
+        <v>166</v>
+      </c>
+      <c r="AC8">
         <v>2.02040041763797E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B9" s="21"/>
       <c r="C9" s="11">
         <v>164</v>
@@ -28646,8 +28997,8 @@
         <v>1.2291530168351701E-2</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -28657,21 +29008,24 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="22"/>
-      <c r="V9">
-        <v>167</v>
-      </c>
-      <c r="W9">
-        <v>1.54108541828033E-2</v>
-      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="22"/>
       <c r="Y9">
         <v>167</v>
       </c>
       <c r="Z9">
+        <v>1.54108541828033E-2</v>
+      </c>
+      <c r="AB9">
+        <v>167</v>
+      </c>
+      <c r="AC9">
         <v>1.9833388018644899E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
       <c r="C10" s="11">
         <v>165</v>
@@ -28687,8 +29041,8 @@
         <v>1.7212899751081399E-2</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -28698,21 +29052,24 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="22"/>
-      <c r="V10">
-        <v>168</v>
-      </c>
-      <c r="W10">
-        <v>1.83994770039482E-2</v>
-      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="22"/>
       <c r="Y10">
         <v>168</v>
       </c>
       <c r="Z10">
+        <v>1.83994770039482E-2</v>
+      </c>
+      <c r="AB10">
+        <v>168</v>
+      </c>
+      <c r="AC10">
         <v>1.77514792876056E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
       <c r="C11" s="11">
         <v>166</v>
@@ -28728,8 +29085,8 @@
         <v>2.02040041763797E-2</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -28739,21 +29096,24 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="22"/>
-      <c r="V11">
-        <v>169</v>
-      </c>
-      <c r="W11">
-        <v>1.8534727187364299E-2</v>
-      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="22"/>
       <c r="Y11">
         <v>169</v>
       </c>
       <c r="Z11">
+        <v>1.8534727187364299E-2</v>
+      </c>
+      <c r="AB11">
+        <v>169</v>
+      </c>
+      <c r="AC11">
         <v>1.92859620408533E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="11">
         <v>167</v>
@@ -28769,8 +29129,8 @@
         <v>1.9833388018644899E-2</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -28780,21 +29140,24 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="22"/>
-      <c r="V12">
-        <v>170</v>
-      </c>
-      <c r="W12">
-        <v>1.85135147784312E-2</v>
-      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="22"/>
       <c r="Y12">
         <v>170</v>
       </c>
       <c r="Z12">
+        <v>1.85135147784312E-2</v>
+      </c>
+      <c r="AB12">
+        <v>170</v>
+      </c>
+      <c r="AC12">
         <v>1.8667112188244999E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="11">
         <v>168</v>
@@ -28810,8 +29173,8 @@
         <v>1.77514792876056E-2</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -28821,21 +29184,24 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="22"/>
-      <c r="V13">
-        <v>171</v>
-      </c>
-      <c r="W13">
-        <v>1.62575809001579E-2</v>
-      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="22"/>
       <c r="Y13">
         <v>171</v>
       </c>
       <c r="Z13">
+        <v>1.62575809001579E-2</v>
+      </c>
+      <c r="AB13">
+        <v>171</v>
+      </c>
+      <c r="AC13">
         <v>1.8649733579546902E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="11">
         <v>169</v>
@@ -28851,8 +29217,8 @@
         <v>1.92859620408533E-2</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -28862,21 +29228,24 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="22"/>
-      <c r="V14">
-        <v>172</v>
-      </c>
-      <c r="W14">
-        <v>1.20891790967672E-2</v>
-      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="22"/>
       <c r="Y14">
         <v>172</v>
       </c>
       <c r="Z14">
+        <v>1.20891790967672E-2</v>
+      </c>
+      <c r="AB14">
+        <v>172</v>
+      </c>
+      <c r="AC14">
         <v>1.71916455869646E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="11">
         <v>170</v>
@@ -28892,8 +29261,8 @@
         <v>1.8667112188244999E-2</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -28903,21 +29272,24 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="22"/>
-      <c r="V15">
-        <v>173</v>
-      </c>
-      <c r="W15">
-        <v>1.5820540470094301E-2</v>
-      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="22"/>
       <c r="Y15">
         <v>173</v>
       </c>
       <c r="Z15">
+        <v>1.5820540470094301E-2</v>
+      </c>
+      <c r="AB15">
+        <v>173</v>
+      </c>
+      <c r="AC15">
         <v>1.28643050115245E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="21"/>
       <c r="C16" s="11">
         <v>171</v>
@@ -28933,8 +29305,8 @@
         <v>1.8649733579546902E-2</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -28944,21 +29316,24 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="22"/>
-      <c r="V16">
-        <v>174</v>
-      </c>
-      <c r="W16">
-        <v>1.30742934372885E-2</v>
-      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="22"/>
       <c r="Y16">
         <v>174</v>
       </c>
       <c r="Z16">
+        <v>1.30742934372885E-2</v>
+      </c>
+      <c r="AB16">
+        <v>174</v>
+      </c>
+      <c r="AC16">
         <v>1.7998364599372398E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
       <c r="C17" s="11">
         <v>172</v>
@@ -28974,8 +29349,8 @@
         <v>1.71916455869646E-2</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -28985,21 +29360,24 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="22"/>
-      <c r="V17">
-        <v>175</v>
-      </c>
-      <c r="W17">
-        <v>2.0212937221922401E-2</v>
-      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="22"/>
       <c r="Y17">
         <v>175</v>
       </c>
       <c r="Z17">
+        <v>2.0212937221922401E-2</v>
+      </c>
+      <c r="AB17">
+        <v>175</v>
+      </c>
+      <c r="AC17">
         <v>1.7850000215170098E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B18" s="21"/>
       <c r="C18" s="11">
         <v>173</v>
@@ -29015,8 +29393,8 @@
         <v>1.28643050115245E-2</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -29026,21 +29404,24 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="22"/>
-      <c r="V18">
-        <v>176</v>
-      </c>
-      <c r="W18">
-        <v>1.25425010247611E-2</v>
-      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="22"/>
       <c r="Y18">
         <v>176</v>
       </c>
       <c r="Z18">
+        <v>1.25425010247611E-2</v>
+      </c>
+      <c r="AB18">
+        <v>176</v>
+      </c>
+      <c r="AC18">
         <v>1.6073409413904699E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B19" s="21"/>
       <c r="C19" s="11">
         <v>174</v>
@@ -29056,8 +29437,8 @@
         <v>1.7998364599372398E-2</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -29067,21 +29448,24 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="22"/>
-      <c r="V19">
-        <v>177</v>
-      </c>
-      <c r="W19">
-        <v>1.8014786805684399E-2</v>
-      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="22"/>
       <c r="Y19">
         <v>177</v>
       </c>
       <c r="Z19">
+        <v>1.8014786805684399E-2</v>
+      </c>
+      <c r="AB19">
+        <v>177</v>
+      </c>
+      <c r="AC19">
         <v>1.78511502583341E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
       <c r="C20" s="11">
         <v>175</v>
@@ -29097,8 +29481,8 @@
         <v>1.7850000215170098E-2</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -29108,21 +29492,24 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="22"/>
-      <c r="V20">
-        <v>178</v>
-      </c>
-      <c r="W20">
-        <v>1.2581674603745799E-2</v>
-      </c>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="22"/>
       <c r="Y20">
         <v>178</v>
       </c>
       <c r="Z20">
+        <v>1.2581674603745799E-2</v>
+      </c>
+      <c r="AB20">
+        <v>178</v>
+      </c>
+      <c r="AC20">
         <v>1.35462800526678E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
       <c r="C21" s="11">
         <v>176</v>
@@ -29138,8 +29525,8 @@
         <v>1.6073409413904699E-2</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -29149,21 +29536,24 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="22"/>
-      <c r="V21">
-        <v>179</v>
-      </c>
-      <c r="W21">
-        <v>1.79359956058209E-2</v>
-      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="22"/>
       <c r="Y21">
         <v>179</v>
       </c>
       <c r="Z21">
+        <v>1.79359956058209E-2</v>
+      </c>
+      <c r="AB21">
+        <v>179</v>
+      </c>
+      <c r="AC21">
         <v>1.30963494850818E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
       <c r="C22" s="11">
         <v>177</v>
@@ -29179,8 +29569,8 @@
         <v>1.78511502583341E-2</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -29190,21 +29580,24 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="22"/>
-      <c r="V22">
-        <v>180</v>
-      </c>
-      <c r="W22">
-        <v>1.34864469971696E-2</v>
-      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="22"/>
       <c r="Y22">
         <v>180</v>
       </c>
       <c r="Z22">
+        <v>1.34864469971696E-2</v>
+      </c>
+      <c r="AB22">
+        <v>180</v>
+      </c>
+      <c r="AC22">
         <v>1.9521480079466701E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B23" s="21"/>
       <c r="C23" s="11">
         <v>178</v>
@@ -29220,8 +29613,8 @@
         <v>1.35462800526678E-2</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -29231,21 +29624,24 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="22"/>
-      <c r="V23">
-        <v>181</v>
-      </c>
-      <c r="W23">
-        <v>1.87375338071907E-2</v>
-      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="22"/>
       <c r="Y23">
         <v>181</v>
       </c>
       <c r="Z23">
+        <v>1.87375338071907E-2</v>
+      </c>
+      <c r="AB23">
+        <v>181</v>
+      </c>
+      <c r="AC23">
         <v>1.6485156962872002E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B24" s="21"/>
       <c r="C24" s="11">
         <v>179</v>
@@ -29261,8 +29657,8 @@
         <v>1.30963494850818E-2</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -29272,21 +29668,24 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="22"/>
-      <c r="V24">
-        <v>182</v>
-      </c>
-      <c r="W24">
-        <v>1.8294268339257E-2</v>
-      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="22"/>
       <c r="Y24">
         <v>182</v>
       </c>
       <c r="Z24">
+        <v>1.8294268339257E-2</v>
+      </c>
+      <c r="AB24">
+        <v>182</v>
+      </c>
+      <c r="AC24">
         <v>1.6667168098000101E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B25" s="21"/>
       <c r="C25" s="11">
         <v>180</v>
@@ -29302,8 +29701,8 @@
         <v>1.9521480079466701E-2</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -29313,21 +29712,24 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="22"/>
-      <c r="V25">
-        <v>183</v>
-      </c>
-      <c r="W25">
-        <v>1.93084358982024E-2</v>
-      </c>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="22"/>
       <c r="Y25">
         <v>183</v>
       </c>
       <c r="Z25">
+        <v>1.93084358982024E-2</v>
+      </c>
+      <c r="AB25">
+        <v>183</v>
+      </c>
+      <c r="AC25">
         <v>1.2843386814332201E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B26" s="21"/>
       <c r="C26" s="11">
         <v>181</v>
@@ -29343,8 +29745,8 @@
         <v>1.6485156962872002E-2</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -29354,21 +29756,24 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="22"/>
-      <c r="V26">
-        <v>184</v>
-      </c>
-      <c r="W26">
-        <v>1.3426578977027599E-2</v>
-      </c>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="22"/>
       <c r="Y26">
         <v>184</v>
       </c>
       <c r="Z26">
+        <v>1.3426578977027599E-2</v>
+      </c>
+      <c r="AB26">
+        <v>184</v>
+      </c>
+      <c r="AC26">
         <v>9.5882367307078605E-3</v>
       </c>
     </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B27" s="21"/>
       <c r="C27" s="11">
         <v>182</v>
@@ -29384,8 +29789,8 @@
         <v>1.6667168098000101E-2</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -29395,21 +29800,24 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="22"/>
-      <c r="V27">
-        <v>185</v>
-      </c>
-      <c r="W27">
-        <v>1.6772511613480201E-2</v>
-      </c>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="22"/>
       <c r="Y27">
         <v>185</v>
       </c>
       <c r="Z27">
+        <v>1.6772511613480201E-2</v>
+      </c>
+      <c r="AB27">
+        <v>185</v>
+      </c>
+      <c r="AC27">
         <v>1.8620013470645101E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B28" s="21"/>
       <c r="C28" s="11">
         <v>183</v>
@@ -29425,8 +29833,8 @@
         <v>1.2843386814332201E-2</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -29436,21 +29844,24 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="22"/>
-      <c r="V28">
-        <v>186</v>
-      </c>
-      <c r="W28">
-        <v>9.5659596456717701E-3</v>
-      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="22"/>
       <c r="Y28">
         <v>186</v>
       </c>
       <c r="Z28">
+        <v>9.5659596456717701E-3</v>
+      </c>
+      <c r="AB28">
+        <v>186</v>
+      </c>
+      <c r="AC28">
         <v>9.8243289322320591E-3</v>
       </c>
     </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B29" s="21"/>
       <c r="C29" s="11">
         <v>184</v>
@@ -29466,8 +29877,8 @@
         <v>9.5882367307078605E-3</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="12"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -29477,21 +29888,24 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="22"/>
-      <c r="V29">
-        <v>187</v>
-      </c>
-      <c r="W29">
-        <v>1.3336194389692401E-2</v>
-      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="22"/>
       <c r="Y29">
         <v>187</v>
       </c>
       <c r="Z29">
+        <v>1.3336194389692401E-2</v>
+      </c>
+      <c r="AB29">
+        <v>187</v>
+      </c>
+      <c r="AC29">
         <v>1.22368320571806E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B30" s="21"/>
       <c r="C30" s="11">
         <v>185</v>
@@ -29507,8 +29921,8 @@
         <v>1.8620013470645101E-2</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="12"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -29518,21 +29932,24 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="22"/>
-      <c r="V30">
-        <v>188</v>
-      </c>
-      <c r="W30">
-        <v>1.88855709357078E-2</v>
-      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="22"/>
       <c r="Y30">
         <v>188</v>
       </c>
       <c r="Z30">
+        <v>1.88855709357078E-2</v>
+      </c>
+      <c r="AB30">
+        <v>188</v>
+      </c>
+      <c r="AC30">
         <v>1.3237362484820899E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B31" s="21"/>
       <c r="C31" s="11">
         <v>186</v>
@@ -29548,8 +29965,8 @@
         <v>9.8243289322320591E-3</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="12"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -29559,21 +29976,24 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-      <c r="T31" s="22"/>
-      <c r="V31">
-        <v>189</v>
-      </c>
-      <c r="W31">
-        <v>1.6842955441203001E-2</v>
-      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="22"/>
       <c r="Y31">
         <v>189</v>
       </c>
       <c r="Z31">
+        <v>1.6842955441203001E-2</v>
+      </c>
+      <c r="AB31">
+        <v>189</v>
+      </c>
+      <c r="AC31">
         <v>1.23195276943599E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B32" s="21"/>
       <c r="C32" s="11">
         <v>187</v>
@@ -29589,8 +30009,8 @@
         <v>1.22368320571806E-2</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -29600,21 +30020,24 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="22"/>
-      <c r="V32">
-        <v>190</v>
-      </c>
-      <c r="W32">
-        <v>1.2684798536274E-2</v>
-      </c>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="22"/>
       <c r="Y32">
         <v>190</v>
       </c>
       <c r="Z32">
+        <v>1.2684798536274E-2</v>
+      </c>
+      <c r="AB32">
+        <v>190</v>
+      </c>
+      <c r="AC32">
         <v>1.1344699668553299E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
       <c r="C33" s="11">
         <v>188</v>
@@ -29630,8 +30053,8 @@
         <v>1.3237362484820899E-2</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="12"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -29641,21 +30064,24 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="22"/>
-      <c r="V33">
-        <v>191</v>
-      </c>
-      <c r="W33">
-        <v>1.78605730833701E-2</v>
-      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="22"/>
       <c r="Y33">
         <v>191</v>
       </c>
       <c r="Z33">
+        <v>1.78605730833701E-2</v>
+      </c>
+      <c r="AB33">
+        <v>191</v>
+      </c>
+      <c r="AC33">
         <v>1.6604778154087198E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B34" s="21"/>
       <c r="C34" s="11">
         <v>189</v>
@@ -29671,8 +30097,8 @@
         <v>1.23195276943599E-2</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="12"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -29682,21 +30108,24 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-      <c r="T34" s="22"/>
-      <c r="V34">
-        <v>192</v>
-      </c>
-      <c r="W34">
-        <v>1.67768916357799E-2</v>
-      </c>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="22"/>
       <c r="Y34">
         <v>192</v>
       </c>
       <c r="Z34">
+        <v>1.67768916357799E-2</v>
+      </c>
+      <c r="AB34">
+        <v>192</v>
+      </c>
+      <c r="AC34">
         <v>9.0634393985407104E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B35" s="21"/>
       <c r="C35" s="11">
         <v>190</v>
@@ -29712,8 +30141,8 @@
         <v>1.1344699668553299E-2</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="12"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -29723,21 +30152,24 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-      <c r="T35" s="22"/>
-      <c r="V35">
-        <v>193</v>
-      </c>
-      <c r="W35">
-        <v>1.7154349734386402E-2</v>
-      </c>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="22"/>
       <c r="Y35">
         <v>193</v>
       </c>
       <c r="Z35">
+        <v>1.7154349734386402E-2</v>
+      </c>
+      <c r="AB35">
+        <v>193</v>
+      </c>
+      <c r="AC35">
         <v>1.7561296204161799E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B36" s="21"/>
       <c r="C36" s="11">
         <v>191</v>
@@ -29753,8 +30185,8 @@
         <v>1.6604778154087198E-2</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="12"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -29764,21 +30196,24 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-      <c r="T36" s="22"/>
-      <c r="V36">
-        <v>194</v>
-      </c>
-      <c r="W36">
-        <v>1.2783720345014699E-2</v>
-      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="22"/>
       <c r="Y36">
         <v>194</v>
       </c>
       <c r="Z36">
+        <v>1.2783720345014699E-2</v>
+      </c>
+      <c r="AB36">
+        <v>194</v>
+      </c>
+      <c r="AC36">
         <v>1.9036057881907899E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B37" s="21"/>
       <c r="C37" s="11">
         <v>192</v>
@@ -29794,8 +30229,8 @@
         <v>9.0634393985407104E-3</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="12"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -29805,21 +30240,24 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="22"/>
-      <c r="V37">
-        <v>195</v>
-      </c>
-      <c r="W37">
-        <v>8.9152729066883998E-3</v>
-      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="22"/>
       <c r="Y37">
         <v>195</v>
       </c>
       <c r="Z37">
+        <v>8.9152729066883998E-3</v>
+      </c>
+      <c r="AB37">
+        <v>195</v>
+      </c>
+      <c r="AC37">
         <v>1.87009922435163E-2</v>
       </c>
     </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B38" s="21"/>
       <c r="C38" s="11">
         <v>193</v>
@@ -29835,8 +30273,8 @@
         <v>1.7561296204161799E-2</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="12"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -29846,21 +30284,24 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
-      <c r="T38" s="22"/>
-      <c r="V38">
-        <v>196</v>
-      </c>
-      <c r="W38">
-        <v>1.5949236635289799E-2</v>
-      </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="22"/>
       <c r="Y38">
         <v>196</v>
       </c>
       <c r="Z38">
+        <v>1.5949236635289799E-2</v>
+      </c>
+      <c r="AB38">
+        <v>196</v>
+      </c>
+      <c r="AC38">
         <v>1.8316731153105201E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B39" s="21"/>
       <c r="C39" s="11">
         <v>194</v>
@@ -29876,8 +30317,8 @@
         <v>1.9036057881907899E-2</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="12"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -29887,21 +30328,24 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
-      <c r="T39" s="22"/>
-      <c r="V39">
-        <v>197</v>
-      </c>
-      <c r="W39">
-        <v>1.15688493740616E-2</v>
-      </c>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="22"/>
       <c r="Y39">
         <v>197</v>
       </c>
       <c r="Z39">
+        <v>1.15688493740616E-2</v>
+      </c>
+      <c r="AB39">
+        <v>197</v>
+      </c>
+      <c r="AC39">
         <v>1.7300714735222399E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B40" s="21"/>
       <c r="C40" s="11">
         <v>195</v>
@@ -29917,8 +30361,8 @@
         <v>1.87009922435163E-2</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="12"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -29928,21 +30372,24 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="22"/>
-      <c r="V40">
-        <v>198</v>
-      </c>
-      <c r="W40">
-        <v>1.7107962974789701E-2</v>
-      </c>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="22"/>
       <c r="Y40">
         <v>198</v>
       </c>
       <c r="Z40">
+        <v>1.7107962974789701E-2</v>
+      </c>
+      <c r="AB40">
+        <v>198</v>
+      </c>
+      <c r="AC40">
         <v>1.36409778698153E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B41" s="21"/>
       <c r="C41" s="11">
         <v>196</v>
@@ -29958,8 +30405,8 @@
         <v>1.8316731153105201E-2</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="12"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -29969,21 +30416,24 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="22"/>
-      <c r="V41">
-        <v>199</v>
-      </c>
-      <c r="W41">
-        <v>1.11965237786554E-2</v>
-      </c>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="22"/>
       <c r="Y41">
         <v>199</v>
       </c>
       <c r="Z41">
+        <v>1.11965237786554E-2</v>
+      </c>
+      <c r="AB41">
+        <v>199</v>
+      </c>
+      <c r="AC41">
         <v>1.11493679766323E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B42" s="21"/>
       <c r="C42" s="11">
         <v>197</v>
@@ -29999,8 +30449,8 @@
         <v>1.7300714735222399E-2</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="12"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -30010,21 +30460,24 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="22"/>
-      <c r="V42">
-        <v>200</v>
-      </c>
-      <c r="W42">
-        <v>9.6007686738408798E-3</v>
-      </c>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="22"/>
       <c r="Y42">
         <v>200</v>
       </c>
       <c r="Z42">
+        <v>9.6007686738408798E-3</v>
+      </c>
+      <c r="AB42">
+        <v>200</v>
+      </c>
+      <c r="AC42">
         <v>1.11949243288769E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B43" s="21"/>
       <c r="C43" s="11">
         <v>198</v>
@@ -30040,8 +30493,8 @@
         <v>1.36409778698153E-2</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="12"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -30051,9 +30504,12 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="22"/>
-    </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="22"/>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B44" s="21"/>
       <c r="C44" s="11">
         <v>199</v>
@@ -30069,8 +30525,8 @@
         <v>1.11493679766323E-2</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="12"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -30080,9 +30536,12 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="22"/>
-    </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="22"/>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B45" s="21"/>
       <c r="C45" s="13">
         <v>200</v>
@@ -30098,8 +30557,8 @@
         <v>1.11949243288769E-2</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -30109,9 +30568,12 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="22"/>
-    </row>
-    <row r="46" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="22"/>
+    </row>
+    <row r="46" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
       <c r="C46" s="24"/>
       <c r="D46" s="25"/>
@@ -30120,7 +30582,7 @@
       <c r="G46" s="25"/>
       <c r="H46" s="24"/>
       <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
+      <c r="J46" s="25"/>
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
@@ -30130,40 +30592,44 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
       <c r="S46" s="24"/>
-      <c r="T46" s="26"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D44">
     <cfRule type="expression" dxfId="18" priority="9">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22:G44">
+  <conditionalFormatting sqref="G22:G44 J22:J26 J40:J44">
     <cfRule type="expression" dxfId="17" priority="8">
       <formula>G22=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:G44">
-    <cfRule type="expression" dxfId="16" priority="7">
+  <conditionalFormatting sqref="G5:G44 J5:J44">
+    <cfRule type="expression" dxfId="0" priority="7">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>D45=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="14" priority="2">
+  <conditionalFormatting sqref="G45 J45">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>G45=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="13" priority="1">
+  <conditionalFormatting sqref="G45 J45">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>G45=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30911,7 +31377,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31992,27 +32458,27 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D36:F36 D38:F41 D37:E37 H36:I41">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>D36=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>D41=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:G33">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>G22=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33825,32 +34291,32 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D44">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22:G44">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>G22=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G44">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>D45=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>G45=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>G45=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33864,8 +34330,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="B1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34598,7 +35064,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Score 4&5 scores and fit
</commit_message>
<xml_diff>
--- a/Documentation/Plots.xlsx
+++ b/Documentation/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/MSE/Cours/MA_BDA/Projet/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CE6955-876E-C74A-8164-FD30A4A3A4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B2DBF0-0C17-7F46-81B3-643CBAD02EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" firstSheet="10" activeTab="17" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19400" firstSheet="10" activeTab="15" xr2:uid="{55D1BBC3-4236-654D-B0EE-A71CC53E19A6}"/>
   </bookViews>
   <sheets>
     <sheet name="clusteringScore0 (20-300)" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="12">
   <si>
     <t>K</t>
   </si>
@@ -506,7 +506,115 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -7076,7 +7184,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'clusteringScore5 (160-200)'!$C$3:$D$3</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$C$3:$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7151,7 +7259,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'clusteringScore5 (160-200)'!$C$5:$C$45</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$C$5:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -7283,132 +7391,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'clusteringScore5 (160-200)'!$D$5:$D$45</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$D$5:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1.10642454992492E-2</c:v>
+                  <c:v>1.8548850592633202E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6093906181799705E-3</c:v>
+                  <c:v>2.0957961831983899E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1345139008171501E-2</c:v>
+                  <c:v>1.37115952998703E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.30485904736607E-2</c:v>
+                  <c:v>1.4286521512344901E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.9068604354760996E-3</c:v>
+                  <c:v>1.91952196167876E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.13533551665545E-2</c:v>
+                  <c:v>1.77636064276235E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1122135490873999E-2</c:v>
+                  <c:v>1.82826836453591E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.3773785694846595E-3</c:v>
+                  <c:v>1.54108541828033E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.6704804791034699E-3</c:v>
+                  <c:v>1.83994770039482E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.7246585702208702E-3</c:v>
+                  <c:v>1.8534727187364299E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.6082163873259102E-3</c:v>
+                  <c:v>1.85135147784312E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0288418839720899E-2</c:v>
+                  <c:v>1.62575809001579E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.1360351715563601E-3</c:v>
+                  <c:v>1.20891790967672E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.7105615620244603E-3</c:v>
+                  <c:v>1.5820540470094301E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.7316447139805598E-3</c:v>
+                  <c:v>1.30742934372885E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.8273799293258808E-3</c:v>
+                  <c:v>2.0212937221922401E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.4153588109838594E-3</c:v>
+                  <c:v>1.25425010247611E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.2355402168959903E-3</c:v>
+                  <c:v>1.8014786805684399E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.9076507182897199E-3</c:v>
+                  <c:v>1.2581674603745799E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0105902251593499E-2</c:v>
+                  <c:v>1.79359956058209E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.0229927320349705E-3</c:v>
+                  <c:v>1.34864469971696E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.5909774503346598E-3</c:v>
+                  <c:v>1.87375338071907E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.3150750420253605E-3</c:v>
+                  <c:v>1.8294268339257E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.5831228792941898E-3</c:v>
+                  <c:v>1.93084358982024E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.6024028502820699E-3</c:v>
+                  <c:v>1.3426578977027599E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.8440701448638699E-3</c:v>
+                  <c:v>1.6772511613480201E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.8404746782488409E-3</c:v>
+                  <c:v>9.5659596456717701E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.5037632769936304E-3</c:v>
+                  <c:v>1.3336194389692401E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.8119311607902598E-3</c:v>
+                  <c:v>1.88855709357078E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.03609121830994E-3</c:v>
+                  <c:v>1.6842955441203001E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.3856748249329493E-3</c:v>
+                  <c:v>1.2684798536274E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.9470535806648902E-3</c:v>
+                  <c:v>1.78605730833701E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.2500051418999002E-3</c:v>
+                  <c:v>1.67768916357799E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.8965899440853801E-3</c:v>
+                  <c:v>1.7154349734386402E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.3268788499191206E-3</c:v>
+                  <c:v>1.2783720345014699E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.8936402919618995E-3</c:v>
+                  <c:v>9.9152729066884007E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.1463346271202306E-3</c:v>
+                  <c:v>1.5949236635289799E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.08938801299191E-2</c:v>
+                  <c:v>1.15688493740616E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.7285003964210697E-3</c:v>
+                  <c:v>1.7107962974789701E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.0108947095604401E-3</c:v>
+                  <c:v>1.11965237786554E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7.50747321598775E-3</c:v>
+                  <c:v>9.6007686738408798E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7416,7 +7524,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-27B5-134C-8F9D-6CD00C9868B7}"/>
+              <c16:uniqueId val="{00000001-B04C-1449-962E-75453E0D15D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7425,7 +7533,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'clusteringScore5 (160-200)'!$F$3:$G$3</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$F$3:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7476,7 +7584,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'clusteringScore5 (160-200)'!$F$5:$F$45</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$F$5:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -7608,132 +7716,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'clusteringScore5 (160-200)'!$G$5:$G$45</c:f>
+              <c:f>'clusteringScore4 (160-200)'!$G$5:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1.02251445059371E-2</c:v>
+                  <c:v>1.73156928908479E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4723624925105399E-3</c:v>
+                  <c:v>1.8384753218102901E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4861070302084492E-3</c:v>
+                  <c:v>1.3799234120787599E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6588888957402597E-3</c:v>
+                  <c:v>1.3864895400583801E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0147295305999094E-3</c:v>
+                  <c:v>1.2291530168351701E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6371390074136394E-3</c:v>
+                  <c:v>1.7212899751081399E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4278296849110399E-2</c:v>
+                  <c:v>2.02040041763797E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.6367096541524703E-3</c:v>
+                  <c:v>1.9833388018644899E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.6196573188000994E-3</c:v>
+                  <c:v>1.77514792876056E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.1140832377963697E-3</c:v>
+                  <c:v>1.92859620408533E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.1346393279152505E-3</c:v>
+                  <c:v>1.8667112188244999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.6753814822897804E-3</c:v>
+                  <c:v>1.8649733579546902E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.3084375013288293E-3</c:v>
+                  <c:v>1.71916455869646E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0616494099436401E-2</c:v>
+                  <c:v>1.28643050115245E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0453306970541001E-2</c:v>
+                  <c:v>1.7998364599372398E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3767481361249298E-3</c:v>
+                  <c:v>1.7850000215170098E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.8644545217441305E-3</c:v>
+                  <c:v>1.6073409413904699E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.03639118713355E-2</c:v>
+                  <c:v>1.78511502583341E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.0030785218174298E-3</c:v>
+                  <c:v>1.35462800526678E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.01069978593536E-2</c:v>
+                  <c:v>1.30963494850818E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.17664132991467E-2</c:v>
+                  <c:v>1.9521480079466701E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.3645591523101997E-3</c:v>
+                  <c:v>1.6485156962872002E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.9132969034983198E-3</c:v>
+                  <c:v>1.6667168098000101E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.8506333701088907E-3</c:v>
+                  <c:v>1.2843386814332201E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.6124545010387498E-3</c:v>
+                  <c:v>9.5882367307078605E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.8138243259799206E-3</c:v>
+                  <c:v>1.8620013470645101E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.2827442994849701E-2</c:v>
+                  <c:v>9.8243289322320591E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.7737831864528204E-3</c:v>
+                  <c:v>1.22368320571806E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.5329780047396896E-3</c:v>
+                  <c:v>1.3237362484820899E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.8905584727450104E-3</c:v>
+                  <c:v>1.23195276943599E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.4470576717168306E-3</c:v>
+                  <c:v>1.1344699668553299E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.9007545346578105E-3</c:v>
+                  <c:v>1.6604778154087198E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.6385489674031205E-3</c:v>
+                  <c:v>9.9634393985407101E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.0023299094900601E-2</c:v>
+                  <c:v>1.7561296204161799E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.66911382025457E-3</c:v>
+                  <c:v>1.9036057881907899E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.4455661291738702E-3</c:v>
+                  <c:v>1.87009922435163E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.8016430209793897E-3</c:v>
+                  <c:v>1.8316731153105201E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>7.7410740622976103E-3</c:v>
+                  <c:v>1.7300714735222399E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.4825002781128101E-3</c:v>
+                  <c:v>1.36409778698153E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.7066886816147297E-3</c:v>
+                  <c:v>1.11493679766323E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5154388149653297E-3</c:v>
+                  <c:v>1.11949243288769E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7741,7 +7849,332 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-27B5-134C-8F9D-6CD00C9868B7}"/>
+              <c16:uniqueId val="{00000003-B04C-1449-962E-75453E0D15D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'clusteringScore4 (160-200)'!$I$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Third run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'clusteringScore4 (160-200)'!$I$5:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'clusteringScore4 (160-200)'!$J$5:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>1.9758252588706799E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.99228148401435E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2722594677179001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1966109999385501E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.92788743934066E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7188191659593899E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.33090669714384E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8900250505117899E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.52331966623938E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.91296444981006E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8876664881661401E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7090653239970801E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.56076995560832E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7633185565659001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8524464085153201E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.29184094987652E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9548622887133799E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8484340678142801E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2095761311904801E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.31520878671049E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.35675253403457E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4834448312789199E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7638188188556399E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.4731484975851092E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0218567456158701E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5223009234116999E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.7932192664336708E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.08547244521105E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4203747636548801E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.6615818081134999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8451379514372999E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.3374638172374E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.23661658354239E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.1642116237256901E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.80456294620512E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2791747334435199E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1782220123410901E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.7853179942490201E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.22610975299956E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.2081078733555401E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.15099390278047E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B04C-1449-962E-75453E0D15D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8639,7 +9072,7 @@
                   </a:schemeClr>
                 </a:solidFill>
               </a:rPr>
-              <a:t>clusteringScore5</a:t>
+              <a:t>clusteringScore4</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -8968,6 +9401,69 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>195</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8977,6 +9473,69 @@
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.26891028702356E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3078497769001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7109871524028399E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.02781232201149E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6296509506035201E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6147161229583401E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5810015095619901E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.15689949576817E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5105817138248099E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5156246825163699E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7064412699316699E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.84174780785996E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.07580128328108E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5512527721222601E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8422442362240901E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6168670944827001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3789475995308E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.26480493476688E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6373147451466299E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.77575115834975E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5809258624735999E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -25369,23 +25928,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E00CB0A1-8E84-B047-B171-9D73F52E101B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167D7CAB-5F17-8D45-9EA3-A4A2AA11A377}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -26910,7 +27469,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="35" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28153,12 +28712,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28906,7 +29465,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29800,12 +30359,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29820,7 +30379,7 @@
   <dimension ref="B1:AF46"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1048576"/>
+      <selection sqref="A1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32176,17 +32735,17 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D45">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>D5=MIN($D$5:$D$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G45">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="18" priority="8">
       <formula>G5=MIN($G$5:$G$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J45">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>J5=MIN($J$5:$J$45)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32934,7 +33493,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34015,12 +34574,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34032,25 +34591,31 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEBE70A3-EFFD-604B-ABCA-B63BD355A6C7}">
   <sheetPr codeName="Sheet16"/>
-  <dimension ref="B1:Z46"/>
+  <dimension ref="B1:AF46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="2.83203125" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="2.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="2.83203125" customWidth="1"/>
-    <col min="20" max="20" width="2.83203125" customWidth="1"/>
-    <col min="24" max="24" width="4" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" customWidth="1"/>
+    <col min="23" max="23" width="2.83203125" customWidth="1"/>
+    <col min="27" max="27" width="4" customWidth="1"/>
+    <col min="30" max="30" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -34069,21 +34634,30 @@
       <c r="Q2" s="19"/>
       <c r="R2" s="19"/>
       <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
-      <c r="V2">
-        <v>160</v>
-      </c>
-      <c r="W2" s="17">
-        <v>1.10642454992492E-2</v>
-      </c>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="20"/>
       <c r="Y2">
         <v>160</v>
       </c>
       <c r="Z2" s="17">
+        <v>1.10642454992492E-2</v>
+      </c>
+      <c r="AB2">
+        <v>160</v>
+      </c>
+      <c r="AC2" s="17">
         <v>1.02251445059371E-2</v>
       </c>
-    </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE2">
+        <v>160</v>
+      </c>
+      <c r="AF2">
+        <v>1.24019132551055E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
       <c r="C3" s="27" t="s">
         <v>4</v>
@@ -34095,8 +34669,10 @@
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -34106,21 +34682,30 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="22"/>
-      <c r="V3">
-        <v>161</v>
-      </c>
-      <c r="W3" s="17">
-        <v>8.6093906181799705E-3</v>
-      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="22"/>
       <c r="Y3">
         <v>161</v>
       </c>
       <c r="Z3" s="17">
+        <v>8.6093906181799705E-3</v>
+      </c>
+      <c r="AB3">
+        <v>161</v>
+      </c>
+      <c r="AC3" s="17">
         <v>8.4723624925105399E-3</v>
       </c>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE3">
+        <v>161</v>
+      </c>
+      <c r="AF3">
+        <v>8.9529372053228102E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4" s="21"/>
       <c r="C4" s="15" t="s">
         <v>0</v>
@@ -34136,8 +34721,12 @@
         <v>1</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>1</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -34147,21 +34736,30 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="22"/>
-      <c r="V4">
-        <v>162</v>
-      </c>
-      <c r="W4" s="17">
-        <v>1.1345139008171501E-2</v>
-      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="22"/>
       <c r="Y4">
         <v>162</v>
       </c>
       <c r="Z4" s="17">
+        <v>1.1345139008171501E-2</v>
+      </c>
+      <c r="AB4">
+        <v>162</v>
+      </c>
+      <c r="AC4" s="17">
         <v>9.4861070302084492E-3</v>
       </c>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE4">
+        <v>162</v>
+      </c>
+      <c r="AF4">
+        <v>1.00693529559152E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
       <c r="C5" s="11">
         <v>160</v>
@@ -34177,8 +34775,12 @@
         <v>1.02251445059371E-2</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="I5" s="11">
+        <v>160</v>
+      </c>
+      <c r="J5" s="12">
+        <v>1.24019132551055E-2</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -34188,21 +34790,30 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="22"/>
-      <c r="V5">
-        <v>163</v>
-      </c>
-      <c r="W5" s="17">
-        <v>1.30485904736607E-2</v>
-      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="22"/>
       <c r="Y5">
         <v>163</v>
       </c>
       <c r="Z5" s="17">
+        <v>1.30485904736607E-2</v>
+      </c>
+      <c r="AB5">
+        <v>163</v>
+      </c>
+      <c r="AC5" s="17">
         <v>8.6588888957402597E-3</v>
       </c>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE5">
+        <v>163</v>
+      </c>
+      <c r="AF5">
+        <v>8.4531987432265206E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B6" s="21"/>
       <c r="C6" s="11">
         <v>161</v>
@@ -34218,8 +34829,12 @@
         <v>8.4723624925105399E-3</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="11">
+        <v>161</v>
+      </c>
+      <c r="J6" s="12">
+        <v>8.9529372053228102E-3</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -34229,21 +34844,30 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="22"/>
-      <c r="V6">
-        <v>164</v>
-      </c>
-      <c r="W6">
-        <v>9.9068604354760996E-3</v>
-      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="22"/>
       <c r="Y6">
         <v>164</v>
       </c>
       <c r="Z6">
+        <v>9.9068604354760996E-3</v>
+      </c>
+      <c r="AB6">
+        <v>164</v>
+      </c>
+      <c r="AC6">
         <v>8.0147295305999094E-3</v>
       </c>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE6">
+        <v>164</v>
+      </c>
+      <c r="AF6">
+        <v>1.0772293065302099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
       <c r="C7" s="11">
         <v>162</v>
@@ -34259,8 +34883,12 @@
         <v>9.4861070302084492E-3</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="11">
+        <v>162</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1.00693529559152E-2</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -34270,21 +34898,30 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="22"/>
-      <c r="V7">
-        <v>165</v>
-      </c>
-      <c r="W7">
-        <v>1.13533551665545E-2</v>
-      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="22"/>
       <c r="Y7">
         <v>165</v>
       </c>
       <c r="Z7">
+        <v>1.13533551665545E-2</v>
+      </c>
+      <c r="AB7">
+        <v>165</v>
+      </c>
+      <c r="AC7">
         <v>8.6371390074136394E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE7">
+        <v>165</v>
+      </c>
+      <c r="AF7">
+        <v>8.5957772582517904E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B8" s="21"/>
       <c r="C8" s="11">
         <v>163</v>
@@ -34300,8 +34937,12 @@
         <v>8.6588888957402597E-3</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="11">
+        <v>163</v>
+      </c>
+      <c r="J8" s="12">
+        <v>8.4531987432265206E-3</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -34311,21 +34952,30 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="22"/>
-      <c r="V8">
-        <v>166</v>
-      </c>
-      <c r="W8">
-        <v>1.1122135490873999E-2</v>
-      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="22"/>
       <c r="Y8">
         <v>166</v>
       </c>
       <c r="Z8">
+        <v>1.1122135490873999E-2</v>
+      </c>
+      <c r="AB8">
+        <v>166</v>
+      </c>
+      <c r="AC8">
         <v>1.4278296849110399E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE8">
+        <v>166</v>
+      </c>
+      <c r="AF8">
+        <v>8.5593974227063298E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B9" s="21"/>
       <c r="C9" s="11">
         <v>164</v>
@@ -34341,8 +34991,12 @@
         <v>8.0147295305999094E-3</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="I9" s="11">
+        <v>164</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1.0772293065302099E-2</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -34352,21 +35006,30 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="22"/>
-      <c r="V9">
-        <v>167</v>
-      </c>
-      <c r="W9">
-        <v>9.3773785694846595E-3</v>
-      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="22"/>
       <c r="Y9">
         <v>167</v>
       </c>
       <c r="Z9">
+        <v>9.3773785694846595E-3</v>
+      </c>
+      <c r="AB9">
+        <v>167</v>
+      </c>
+      <c r="AC9">
         <v>9.6367096541524703E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE9">
+        <v>167</v>
+      </c>
+      <c r="AF9">
+        <v>1.15902944184786E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
       <c r="C10" s="11">
         <v>165</v>
@@ -34382,8 +35045,12 @@
         <v>8.6371390074136394E-3</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="11">
+        <v>165</v>
+      </c>
+      <c r="J10" s="12">
+        <v>8.5957772582517904E-3</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -34393,21 +35060,30 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="22"/>
-      <c r="V10">
-        <v>168</v>
-      </c>
-      <c r="W10">
-        <v>8.6704804791034699E-3</v>
-      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="22"/>
       <c r="Y10">
         <v>168</v>
       </c>
       <c r="Z10">
+        <v>8.6704804791034699E-3</v>
+      </c>
+      <c r="AB10">
+        <v>168</v>
+      </c>
+      <c r="AC10">
         <v>9.6196573188000994E-3</v>
       </c>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE10">
+        <v>168</v>
+      </c>
+      <c r="AF10">
+        <v>1.4427544065673001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
       <c r="C11" s="11">
         <v>166</v>
@@ -34423,8 +35099,12 @@
         <v>1.4278296849110399E-2</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="11">
+        <v>166</v>
+      </c>
+      <c r="J11" s="12">
+        <v>8.5593974227063298E-3</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -34434,21 +35114,30 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="22"/>
-      <c r="V11">
-        <v>169</v>
-      </c>
-      <c r="W11">
-        <v>8.7246585702208702E-3</v>
-      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="22"/>
       <c r="Y11">
         <v>169</v>
       </c>
       <c r="Z11">
+        <v>8.7246585702208702E-3</v>
+      </c>
+      <c r="AB11">
+        <v>169</v>
+      </c>
+      <c r="AC11">
         <v>9.1140832377963697E-3</v>
       </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE11">
+        <v>169</v>
+      </c>
+      <c r="AF11">
+        <v>8.6081000394951906E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
       <c r="C12" s="11">
         <v>167</v>
@@ -34464,8 +35153,12 @@
         <v>9.6367096541524703E-3</v>
       </c>
       <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="I12" s="11">
+        <v>167</v>
+      </c>
+      <c r="J12" s="12">
+        <v>1.15902944184786E-2</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -34475,21 +35168,30 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="22"/>
-      <c r="V12">
-        <v>170</v>
-      </c>
-      <c r="W12">
-        <v>7.6082163873259102E-3</v>
-      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="22"/>
       <c r="Y12">
         <v>170</v>
       </c>
       <c r="Z12">
+        <v>7.6082163873259102E-3</v>
+      </c>
+      <c r="AB12">
+        <v>170</v>
+      </c>
+      <c r="AC12">
         <v>9.1346393279152505E-3</v>
       </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE12">
+        <v>170</v>
+      </c>
+      <c r="AF12">
+        <v>1.5111261936567401E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
       <c r="C13" s="11">
         <v>168</v>
@@ -34505,8 +35207,12 @@
         <v>9.6196573188000994E-3</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="I13" s="11">
+        <v>168</v>
+      </c>
+      <c r="J13" s="12">
+        <v>1.4427544065673001E-2</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -34516,21 +35222,30 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="22"/>
-      <c r="V13">
-        <v>171</v>
-      </c>
-      <c r="W13">
-        <v>1.0288418839720899E-2</v>
-      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="22"/>
       <c r="Y13">
         <v>171</v>
       </c>
       <c r="Z13">
+        <v>1.0288418839720899E-2</v>
+      </c>
+      <c r="AB13">
+        <v>171</v>
+      </c>
+      <c r="AC13">
         <v>8.6753814822897804E-3</v>
       </c>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE13">
+        <v>171</v>
+      </c>
+      <c r="AF13">
+        <v>9.4052459484654394E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
       <c r="C14" s="11">
         <v>169</v>
@@ -34546,8 +35261,12 @@
         <v>9.1140832377963697E-3</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="I14" s="11">
+        <v>169</v>
+      </c>
+      <c r="J14" s="12">
+        <v>8.6081000394951906E-3</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -34557,21 +35276,30 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="22"/>
-      <c r="V14">
-        <v>172</v>
-      </c>
-      <c r="W14">
-        <v>9.1360351715563601E-3</v>
-      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="22"/>
       <c r="Y14">
         <v>172</v>
       </c>
       <c r="Z14">
+        <v>9.1360351715563601E-3</v>
+      </c>
+      <c r="AB14">
+        <v>172</v>
+      </c>
+      <c r="AC14">
         <v>8.3084375013288293E-3</v>
       </c>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE14">
+        <v>172</v>
+      </c>
+      <c r="AF14">
+        <v>9.2807381740704301E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
       <c r="C15" s="11">
         <v>170</v>
@@ -34587,8 +35315,12 @@
         <v>9.1346393279152505E-3</v>
       </c>
       <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="I15" s="11">
+        <v>170</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1.5111261936567401E-2</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -34598,21 +35330,30 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="22"/>
-      <c r="V15">
-        <v>173</v>
-      </c>
-      <c r="W15">
-        <v>7.7105615620244603E-3</v>
-      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="22"/>
       <c r="Y15">
         <v>173</v>
       </c>
       <c r="Z15">
+        <v>7.7105615620244603E-3</v>
+      </c>
+      <c r="AB15">
+        <v>173</v>
+      </c>
+      <c r="AC15">
         <v>1.0616494099436401E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE15">
+        <v>173</v>
+      </c>
+      <c r="AF15">
+        <v>9.4295025910777798E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B16" s="21"/>
       <c r="C16" s="11">
         <v>171</v>
@@ -34628,8 +35369,12 @@
         <v>8.6753814822897804E-3</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="11">
+        <v>171</v>
+      </c>
+      <c r="J16" s="12">
+        <v>9.4052459484654394E-3</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -34639,21 +35384,30 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="22"/>
-      <c r="V16">
-        <v>174</v>
-      </c>
-      <c r="W16">
-        <v>7.7316447139805598E-3</v>
-      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="22"/>
       <c r="Y16">
         <v>174</v>
       </c>
       <c r="Z16">
+        <v>7.7316447139805598E-3</v>
+      </c>
+      <c r="AB16">
+        <v>174</v>
+      </c>
+      <c r="AC16">
         <v>1.0453306970541001E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE16">
+        <v>174</v>
+      </c>
+      <c r="AF16">
+        <v>9.4274722606251804E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
       <c r="C17" s="11">
         <v>172</v>
@@ -34669,8 +35423,12 @@
         <v>8.3084375013288293E-3</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="I17" s="11">
+        <v>172</v>
+      </c>
+      <c r="J17" s="12">
+        <v>9.2807381740704301E-3</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -34680,21 +35438,30 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="22"/>
-      <c r="V17">
-        <v>175</v>
-      </c>
-      <c r="W17">
-        <v>7.8273799293258808E-3</v>
-      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="22"/>
       <c r="Y17">
         <v>175</v>
       </c>
       <c r="Z17">
+        <v>7.8273799293258808E-3</v>
+      </c>
+      <c r="AB17">
+        <v>175</v>
+      </c>
+      <c r="AC17">
         <v>9.3767481361249298E-3</v>
       </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE17">
+        <v>175</v>
+      </c>
+      <c r="AF17">
+        <v>9.2264464385115996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B18" s="21"/>
       <c r="C18" s="11">
         <v>173</v>
@@ -34710,8 +35477,12 @@
         <v>1.0616494099436401E-2</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="I18" s="11">
+        <v>173</v>
+      </c>
+      <c r="J18" s="12">
+        <v>9.4295025910777798E-3</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -34721,21 +35492,30 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="22"/>
-      <c r="V18">
-        <v>176</v>
-      </c>
-      <c r="W18">
-        <v>8.4153588109838594E-3</v>
-      </c>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="22"/>
       <c r="Y18">
         <v>176</v>
       </c>
       <c r="Z18">
+        <v>8.4153588109838594E-3</v>
+      </c>
+      <c r="AB18">
+        <v>176</v>
+      </c>
+      <c r="AC18">
         <v>9.8644545217441305E-3</v>
       </c>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE18">
+        <v>176</v>
+      </c>
+      <c r="AF18">
+        <v>9.2761061755464898E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B19" s="21"/>
       <c r="C19" s="11">
         <v>174</v>
@@ -34751,8 +35531,12 @@
         <v>1.0453306970541001E-2</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="I19" s="11">
+        <v>174</v>
+      </c>
+      <c r="J19" s="12">
+        <v>9.4274722606251804E-3</v>
+      </c>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -34762,21 +35546,30 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="22"/>
-      <c r="V19">
-        <v>177</v>
-      </c>
-      <c r="W19">
-        <v>8.2355402168959903E-3</v>
-      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="22"/>
       <c r="Y19">
         <v>177</v>
       </c>
       <c r="Z19">
+        <v>8.2355402168959903E-3</v>
+      </c>
+      <c r="AB19">
+        <v>177</v>
+      </c>
+      <c r="AC19">
         <v>1.03639118713355E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE19">
+        <v>177</v>
+      </c>
+      <c r="AF19">
+        <v>8.3585748834712308E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
       <c r="C20" s="11">
         <v>175</v>
@@ -34792,8 +35585,12 @@
         <v>9.3767481361249298E-3</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="I20" s="11">
+        <v>175</v>
+      </c>
+      <c r="J20" s="12">
+        <v>9.2264464385115996E-3</v>
+      </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -34803,21 +35600,30 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="22"/>
-      <c r="V20">
-        <v>178</v>
-      </c>
-      <c r="W20">
-        <v>9.9076507182897199E-3</v>
-      </c>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="22"/>
       <c r="Y20">
         <v>178</v>
       </c>
       <c r="Z20">
+        <v>9.9076507182897199E-3</v>
+      </c>
+      <c r="AB20">
+        <v>178</v>
+      </c>
+      <c r="AC20">
         <v>7.0030785218174298E-3</v>
       </c>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE20">
+        <v>178</v>
+      </c>
+      <c r="AF20">
+        <v>6.9835839179156999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
       <c r="C21" s="11">
         <v>176</v>
@@ -34833,8 +35639,12 @@
         <v>9.8644545217441305E-3</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="I21" s="11">
+        <v>176</v>
+      </c>
+      <c r="J21" s="12">
+        <v>9.2761061755464898E-3</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -34844,21 +35654,30 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="22"/>
-      <c r="V21">
-        <v>179</v>
-      </c>
-      <c r="W21">
-        <v>1.0105902251593499E-2</v>
-      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="22"/>
       <c r="Y21">
         <v>179</v>
       </c>
       <c r="Z21">
+        <v>1.0105902251593499E-2</v>
+      </c>
+      <c r="AB21">
+        <v>179</v>
+      </c>
+      <c r="AC21">
         <v>1.01069978593536E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE21">
+        <v>179</v>
+      </c>
+      <c r="AF21">
+        <v>9.3161739957089706E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
       <c r="C22" s="11">
         <v>177</v>
@@ -34874,8 +35693,12 @@
         <v>1.03639118713355E-2</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="I22" s="11">
+        <v>177</v>
+      </c>
+      <c r="J22" s="12">
+        <v>8.3585748834712308E-3</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -34885,21 +35708,30 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="22"/>
-      <c r="V22">
-        <v>180</v>
-      </c>
-      <c r="W22">
-        <v>8.0229927320349705E-3</v>
-      </c>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="22"/>
       <c r="Y22">
         <v>180</v>
       </c>
       <c r="Z22">
+        <v>8.0229927320349705E-3</v>
+      </c>
+      <c r="AB22">
+        <v>180</v>
+      </c>
+      <c r="AC22">
         <v>1.17664132991467E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE22">
+        <v>180</v>
+      </c>
+      <c r="AF22">
+        <v>7.0786114861580898E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B23" s="21"/>
       <c r="C23" s="11">
         <v>178</v>
@@ -34915,8 +35747,12 @@
         <v>7.0030785218174298E-3</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="I23" s="11">
+        <v>178</v>
+      </c>
+      <c r="J23" s="12">
+        <v>6.9835839179156999E-3</v>
+      </c>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -34926,21 +35762,30 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="22"/>
-      <c r="V23">
-        <v>181</v>
-      </c>
-      <c r="W23">
-        <v>7.5909774503346598E-3</v>
-      </c>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="22"/>
       <c r="Y23">
         <v>181</v>
       </c>
       <c r="Z23">
+        <v>7.5909774503346598E-3</v>
+      </c>
+      <c r="AB23">
+        <v>181</v>
+      </c>
+      <c r="AC23">
         <v>7.3645591523101997E-3</v>
       </c>
-    </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE23">
+        <v>181</v>
+      </c>
+      <c r="AF23">
+        <v>9.5036406725882098E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B24" s="21"/>
       <c r="C24" s="11">
         <v>179</v>
@@ -34956,8 +35801,12 @@
         <v>1.01069978593536E-2</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="I24" s="11">
+        <v>179</v>
+      </c>
+      <c r="J24" s="12">
+        <v>9.3161739957089706E-3</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -34967,21 +35816,30 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="22"/>
-      <c r="V24">
-        <v>182</v>
-      </c>
-      <c r="W24">
-        <v>8.3150750420253605E-3</v>
-      </c>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="22"/>
       <c r="Y24">
         <v>182</v>
       </c>
       <c r="Z24">
+        <v>8.3150750420253605E-3</v>
+      </c>
+      <c r="AB24">
+        <v>182</v>
+      </c>
+      <c r="AC24">
         <v>9.9132969034983198E-3</v>
       </c>
-    </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE24">
+        <v>182</v>
+      </c>
+      <c r="AF24">
+        <v>8.0580748540373306E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B25" s="21"/>
       <c r="C25" s="11">
         <v>180</v>
@@ -34997,8 +35855,12 @@
         <v>1.17664132991467E-2</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="I25" s="11">
+        <v>180</v>
+      </c>
+      <c r="J25" s="12">
+        <v>7.0786114861580898E-3</v>
+      </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -35008,21 +35870,30 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="22"/>
-      <c r="V25">
-        <v>183</v>
-      </c>
-      <c r="W25">
-        <v>7.5831228792941898E-3</v>
-      </c>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="22"/>
       <c r="Y25">
         <v>183</v>
       </c>
       <c r="Z25">
+        <v>7.5831228792941898E-3</v>
+      </c>
+      <c r="AB25">
+        <v>183</v>
+      </c>
+      <c r="AC25">
         <v>7.8506333701088907E-3</v>
       </c>
-    </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE25">
+        <v>183</v>
+      </c>
+      <c r="AF25">
+        <v>8.4424708816048903E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B26" s="21"/>
       <c r="C26" s="11">
         <v>181</v>
@@ -35038,8 +35909,12 @@
         <v>7.3645591523101997E-3</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="I26" s="11">
+        <v>181</v>
+      </c>
+      <c r="J26" s="12">
+        <v>9.5036406725882098E-3</v>
+      </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -35049,21 +35924,30 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="22"/>
-      <c r="V26">
-        <v>184</v>
-      </c>
-      <c r="W26">
-        <v>7.6024028502820699E-3</v>
-      </c>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="22"/>
       <c r="Y26">
         <v>184</v>
       </c>
       <c r="Z26">
+        <v>7.6024028502820699E-3</v>
+      </c>
+      <c r="AB26">
+        <v>184</v>
+      </c>
+      <c r="AC26">
         <v>7.6124545010387498E-3</v>
       </c>
-    </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE26">
+        <v>184</v>
+      </c>
+      <c r="AF26">
+        <v>8.4721092489708598E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B27" s="21"/>
       <c r="C27" s="11">
         <v>182</v>
@@ -35079,8 +35963,12 @@
         <v>9.9132969034983198E-3</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="I27" s="11">
+        <v>182</v>
+      </c>
+      <c r="J27" s="12">
+        <v>8.0580748540373306E-3</v>
+      </c>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -35090,21 +35978,30 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-      <c r="T27" s="22"/>
-      <c r="V27">
-        <v>185</v>
-      </c>
-      <c r="W27">
-        <v>8.8440701448638699E-3</v>
-      </c>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="22"/>
       <c r="Y27">
         <v>185</v>
       </c>
       <c r="Z27">
+        <v>8.8440701448638699E-3</v>
+      </c>
+      <c r="AB27">
+        <v>185</v>
+      </c>
+      <c r="AC27">
         <v>7.8138243259799206E-3</v>
       </c>
-    </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE27">
+        <v>185</v>
+      </c>
+      <c r="AF27">
+        <v>7.0201626578968602E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B28" s="21"/>
       <c r="C28" s="11">
         <v>183</v>
@@ -35120,8 +36017,12 @@
         <v>7.8506333701088907E-3</v>
       </c>
       <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="I28" s="11">
+        <v>183</v>
+      </c>
+      <c r="J28" s="12">
+        <v>8.4424708816048903E-3</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -35131,21 +36032,30 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-      <c r="T28" s="22"/>
-      <c r="V28">
-        <v>186</v>
-      </c>
-      <c r="W28">
-        <v>9.8404746782488409E-3</v>
-      </c>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="22"/>
       <c r="Y28">
         <v>186</v>
       </c>
       <c r="Z28">
+        <v>9.8404746782488409E-3</v>
+      </c>
+      <c r="AB28">
+        <v>186</v>
+      </c>
+      <c r="AC28">
         <v>1.2827442994849701E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE28">
+        <v>186</v>
+      </c>
+      <c r="AF28">
+        <v>9.3580431772930101E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B29" s="21"/>
       <c r="C29" s="11">
         <v>184</v>
@@ -35161,8 +36071,12 @@
         <v>7.6124545010387498E-3</v>
       </c>
       <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="I29" s="11">
+        <v>184</v>
+      </c>
+      <c r="J29" s="12">
+        <v>8.4721092489708598E-3</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -35172,21 +36086,30 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-      <c r="T29" s="22"/>
-      <c r="V29">
-        <v>187</v>
-      </c>
-      <c r="W29">
-        <v>7.5037632769936304E-3</v>
-      </c>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="22"/>
       <c r="Y29">
         <v>187</v>
       </c>
       <c r="Z29">
+        <v>7.5037632769936304E-3</v>
+      </c>
+      <c r="AB29">
+        <v>187</v>
+      </c>
+      <c r="AC29">
         <v>5.7737831864528204E-3</v>
       </c>
-    </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE29">
+        <v>187</v>
+      </c>
+      <c r="AF29">
+        <v>6.6746068321478901E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B30" s="21"/>
       <c r="C30" s="11">
         <v>185</v>
@@ -35202,8 +36125,12 @@
         <v>7.8138243259799206E-3</v>
       </c>
       <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="I30" s="11">
+        <v>185</v>
+      </c>
+      <c r="J30" s="12">
+        <v>7.0201626578968602E-3</v>
+      </c>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -35213,21 +36140,30 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-      <c r="T30" s="22"/>
-      <c r="V30">
-        <v>188</v>
-      </c>
-      <c r="W30">
-        <v>7.8119311607902598E-3</v>
-      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="22"/>
       <c r="Y30">
         <v>188</v>
       </c>
       <c r="Z30">
+        <v>7.8119311607902598E-3</v>
+      </c>
+      <c r="AB30">
+        <v>188</v>
+      </c>
+      <c r="AC30">
         <v>7.5329780047396896E-3</v>
       </c>
-    </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE30">
+        <v>188</v>
+      </c>
+      <c r="AF30">
+        <v>7.4226925849101297E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B31" s="21"/>
       <c r="C31" s="11">
         <v>186</v>
@@ -35243,8 +36179,12 @@
         <v>1.2827442994849701E-2</v>
       </c>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="I31" s="11">
+        <v>186</v>
+      </c>
+      <c r="J31" s="12">
+        <v>9.3580431772930101E-3</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -35254,21 +36194,30 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-      <c r="T31" s="22"/>
-      <c r="V31">
-        <v>189</v>
-      </c>
-      <c r="W31">
-        <v>8.03609121830994E-3</v>
-      </c>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="22"/>
       <c r="Y31">
         <v>189</v>
       </c>
       <c r="Z31">
+        <v>8.03609121830994E-3</v>
+      </c>
+      <c r="AB31">
+        <v>189</v>
+      </c>
+      <c r="AC31">
         <v>7.8905584727450104E-3</v>
       </c>
-    </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE31">
+        <v>189</v>
+      </c>
+      <c r="AF31">
+        <v>6.8487787527760297E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B32" s="21"/>
       <c r="C32" s="11">
         <v>187</v>
@@ -35284,8 +36233,12 @@
         <v>5.7737831864528204E-3</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="I32" s="11">
+        <v>187</v>
+      </c>
+      <c r="J32" s="12">
+        <v>6.6746068321478901E-3</v>
+      </c>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -35295,21 +36248,30 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="22"/>
-      <c r="V32">
-        <v>190</v>
-      </c>
-      <c r="W32">
-        <v>8.3856748249329493E-3</v>
-      </c>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="22"/>
       <c r="Y32">
         <v>190</v>
       </c>
       <c r="Z32">
+        <v>8.3856748249329493E-3</v>
+      </c>
+      <c r="AB32">
+        <v>190</v>
+      </c>
+      <c r="AC32">
         <v>8.4470576717168306E-3</v>
       </c>
-    </row>
-    <row r="33" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE32">
+        <v>190</v>
+      </c>
+      <c r="AF32">
+        <v>7.2246004357826698E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B33" s="21"/>
       <c r="C33" s="11">
         <v>188</v>
@@ -35325,8 +36287,12 @@
         <v>7.5329780047396896E-3</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
+      <c r="I33" s="11">
+        <v>188</v>
+      </c>
+      <c r="J33" s="12">
+        <v>7.4226925849101297E-3</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -35336,21 +36302,30 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="22"/>
-      <c r="V33">
-        <v>191</v>
-      </c>
-      <c r="W33">
-        <v>7.9470535806648902E-3</v>
-      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="22"/>
       <c r="Y33">
         <v>191</v>
       </c>
       <c r="Z33">
+        <v>7.9470535806648902E-3</v>
+      </c>
+      <c r="AB33">
+        <v>191</v>
+      </c>
+      <c r="AC33">
         <v>7.9007545346578105E-3</v>
       </c>
-    </row>
-    <row r="34" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE33">
+        <v>191</v>
+      </c>
+      <c r="AF33">
+        <v>1.01996238610591E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B34" s="21"/>
       <c r="C34" s="11">
         <v>189</v>
@@ -35366,8 +36341,12 @@
         <v>7.8905584727450104E-3</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
+      <c r="I34" s="11">
+        <v>189</v>
+      </c>
+      <c r="J34" s="12">
+        <v>6.8487787527760297E-3</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -35377,21 +36356,30 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-      <c r="T34" s="22"/>
-      <c r="V34">
-        <v>192</v>
-      </c>
-      <c r="W34">
-        <v>9.2500051418999002E-3</v>
-      </c>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="22"/>
       <c r="Y34">
         <v>192</v>
       </c>
       <c r="Z34">
+        <v>9.2500051418999002E-3</v>
+      </c>
+      <c r="AB34">
+        <v>192</v>
+      </c>
+      <c r="AC34">
         <v>8.6385489674031205E-3</v>
       </c>
-    </row>
-    <row r="35" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE34">
+        <v>192</v>
+      </c>
+      <c r="AF34">
+        <v>6.99478885838903E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B35" s="21"/>
       <c r="C35" s="11">
         <v>190</v>
@@ -35407,8 +36395,12 @@
         <v>8.4470576717168306E-3</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="I35" s="11">
+        <v>190</v>
+      </c>
+      <c r="J35" s="12">
+        <v>7.2246004357826698E-3</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -35418,21 +36410,30 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-      <c r="T35" s="22"/>
-      <c r="V35">
-        <v>193</v>
-      </c>
-      <c r="W35">
-        <v>7.8965899440853801E-3</v>
-      </c>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="22"/>
       <c r="Y35">
         <v>193</v>
       </c>
       <c r="Z35">
+        <v>7.8965899440853801E-3</v>
+      </c>
+      <c r="AB35">
+        <v>193</v>
+      </c>
+      <c r="AC35">
         <v>1.0023299094900601E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE35">
+        <v>193</v>
+      </c>
+      <c r="AF35">
+        <v>7.2129824677651597E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B36" s="21"/>
       <c r="C36" s="11">
         <v>191</v>
@@ -35448,8 +36449,12 @@
         <v>7.9007545346578105E-3</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
+      <c r="I36" s="11">
+        <v>191</v>
+      </c>
+      <c r="J36" s="12">
+        <v>1.01996238610591E-2</v>
+      </c>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -35459,21 +36464,30 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-      <c r="T36" s="22"/>
-      <c r="V36">
-        <v>194</v>
-      </c>
-      <c r="W36">
-        <v>8.3268788499191206E-3</v>
-      </c>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="22"/>
       <c r="Y36">
         <v>194</v>
       </c>
       <c r="Z36">
+        <v>8.3268788499191206E-3</v>
+      </c>
+      <c r="AB36">
+        <v>194</v>
+      </c>
+      <c r="AC36">
         <v>7.66911382025457E-3</v>
       </c>
-    </row>
-    <row r="37" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE36">
+        <v>194</v>
+      </c>
+      <c r="AF36">
+        <v>7.6032868544863297E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B37" s="21"/>
       <c r="C37" s="11">
         <v>192</v>
@@ -35489,8 +36503,12 @@
         <v>8.6385489674031205E-3</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
+      <c r="I37" s="11">
+        <v>192</v>
+      </c>
+      <c r="J37" s="12">
+        <v>6.99478885838903E-3</v>
+      </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -35500,21 +36518,30 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-      <c r="T37" s="22"/>
-      <c r="V37">
-        <v>195</v>
-      </c>
-      <c r="W37">
-        <v>7.8936402919618995E-3</v>
-      </c>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="22"/>
       <c r="Y37">
         <v>195</v>
       </c>
       <c r="Z37">
+        <v>7.8936402919618995E-3</v>
+      </c>
+      <c r="AB37">
+        <v>195</v>
+      </c>
+      <c r="AC37">
         <v>7.4455661291738702E-3</v>
       </c>
-    </row>
-    <row r="38" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE37">
+        <v>195</v>
+      </c>
+      <c r="AF37">
+        <v>7.2310326224340003E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B38" s="21"/>
       <c r="C38" s="11">
         <v>193</v>
@@ -35530,8 +36557,12 @@
         <v>1.0023299094900601E-2</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
+      <c r="I38" s="11">
+        <v>193</v>
+      </c>
+      <c r="J38" s="12">
+        <v>7.2129824677651597E-3</v>
+      </c>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -35541,21 +36572,30 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
-      <c r="T38" s="22"/>
-      <c r="V38">
-        <v>196</v>
-      </c>
-      <c r="W38">
-        <v>8.1463346271202306E-3</v>
-      </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="22"/>
       <c r="Y38">
         <v>196</v>
       </c>
       <c r="Z38">
+        <v>8.1463346271202306E-3</v>
+      </c>
+      <c r="AB38">
+        <v>196</v>
+      </c>
+      <c r="AC38">
         <v>8.8016430209793897E-3</v>
       </c>
-    </row>
-    <row r="39" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE38">
+        <v>196</v>
+      </c>
+      <c r="AF38">
+        <v>6.9660783273169597E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B39" s="21"/>
       <c r="C39" s="11">
         <v>194</v>
@@ -35571,8 +36611,12 @@
         <v>7.66911382025457E-3</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
+      <c r="I39" s="11">
+        <v>194</v>
+      </c>
+      <c r="J39" s="12">
+        <v>7.6032868544863297E-3</v>
+      </c>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -35582,21 +36626,30 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
-      <c r="T39" s="22"/>
-      <c r="V39">
-        <v>197</v>
-      </c>
-      <c r="W39">
-        <v>1.08938801299191E-2</v>
-      </c>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="22"/>
       <c r="Y39">
         <v>197</v>
       </c>
       <c r="Z39">
+        <v>1.08938801299191E-2</v>
+      </c>
+      <c r="AB39">
+        <v>197</v>
+      </c>
+      <c r="AC39">
         <v>7.7410740622976103E-3</v>
       </c>
-    </row>
-    <row r="40" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE39">
+        <v>197</v>
+      </c>
+      <c r="AF39">
+        <v>7.1569710635546596E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B40" s="21"/>
       <c r="C40" s="11">
         <v>195</v>
@@ -35612,8 +36665,12 @@
         <v>7.4455661291738702E-3</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
+      <c r="I40" s="11">
+        <v>195</v>
+      </c>
+      <c r="J40" s="12">
+        <v>7.2310326224340003E-3</v>
+      </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -35623,21 +36680,30 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
-      <c r="T40" s="22"/>
-      <c r="V40">
-        <v>198</v>
-      </c>
-      <c r="W40">
-        <v>8.7285003964210697E-3</v>
-      </c>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="22"/>
       <c r="Y40">
         <v>198</v>
       </c>
       <c r="Z40">
+        <v>8.7285003964210697E-3</v>
+      </c>
+      <c r="AB40">
+        <v>198</v>
+      </c>
+      <c r="AC40">
         <v>7.4825002781128101E-3</v>
       </c>
-    </row>
-    <row r="41" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE40">
+        <v>198</v>
+      </c>
+      <c r="AF40">
+        <v>1.0019199224448201E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B41" s="21"/>
       <c r="C41" s="11">
         <v>196</v>
@@ -35653,8 +36719,12 @@
         <v>8.8016430209793897E-3</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
+      <c r="I41" s="11">
+        <v>196</v>
+      </c>
+      <c r="J41" s="12">
+        <v>6.9660783273169597E-3</v>
+      </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -35664,21 +36734,30 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
-      <c r="T41" s="22"/>
-      <c r="V41">
-        <v>199</v>
-      </c>
-      <c r="W41">
-        <v>9.0108947095604401E-3</v>
-      </c>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="22"/>
       <c r="Y41">
         <v>199</v>
       </c>
       <c r="Z41">
+        <v>9.0108947095604401E-3</v>
+      </c>
+      <c r="AB41">
+        <v>199</v>
+      </c>
+      <c r="AC41">
         <v>7.7066886816147297E-3</v>
       </c>
-    </row>
-    <row r="42" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE41">
+        <v>199</v>
+      </c>
+      <c r="AF41">
+        <v>6.8165720640501401E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B42" s="21"/>
       <c r="C42" s="11">
         <v>197</v>
@@ -35694,8 +36773,12 @@
         <v>7.7410740622976103E-3</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
+      <c r="I42" s="11">
+        <v>197</v>
+      </c>
+      <c r="J42" s="12">
+        <v>7.1569710635546596E-3</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -35705,21 +36788,30 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-      <c r="T42" s="22"/>
-      <c r="V42">
-        <v>200</v>
-      </c>
-      <c r="W42">
-        <v>7.50747321598775E-3</v>
-      </c>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="22"/>
       <c r="Y42">
         <v>200</v>
       </c>
       <c r="Z42">
+        <v>7.50747321598775E-3</v>
+      </c>
+      <c r="AB42">
+        <v>200</v>
+      </c>
+      <c r="AC42">
         <v>6.5154388149653297E-3</v>
       </c>
-    </row>
-    <row r="43" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="AE42">
+        <v>200</v>
+      </c>
+      <c r="AF42">
+        <v>7.0374274578216597E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B43" s="21"/>
       <c r="C43" s="11">
         <v>198</v>
@@ -35735,8 +36827,12 @@
         <v>7.4825002781128101E-3</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
+      <c r="I43" s="11">
+        <v>198</v>
+      </c>
+      <c r="J43" s="12">
+        <v>1.0019199224448201E-2</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -35746,9 +36842,12 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="22"/>
-    </row>
-    <row r="44" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="22"/>
+    </row>
+    <row r="44" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B44" s="21"/>
       <c r="C44" s="11">
         <v>199</v>
@@ -35764,8 +36863,12 @@
         <v>7.7066886816147297E-3</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
+      <c r="I44" s="11">
+        <v>199</v>
+      </c>
+      <c r="J44" s="12">
+        <v>6.8165720640501401E-3</v>
+      </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -35775,9 +36878,12 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="22"/>
-    </row>
-    <row r="45" spans="2:26" x14ac:dyDescent="0.2">
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="22"/>
+    </row>
+    <row r="45" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B45" s="21"/>
       <c r="C45" s="13">
         <v>200</v>
@@ -35793,8 +36899,12 @@
         <v>6.5154388149653297E-3</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
+      <c r="I45" s="13">
+        <v>200</v>
+      </c>
+      <c r="J45" s="14">
+        <v>7.0374274578216597E-3</v>
+      </c>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -35804,9 +36914,12 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="22"/>
-    </row>
-    <row r="46" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="22"/>
+    </row>
+    <row r="46" spans="2:32" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
       <c r="C46" s="24"/>
       <c r="D46" s="25"/>
@@ -35815,7 +36928,7 @@
       <c r="G46" s="25"/>
       <c r="H46" s="24"/>
       <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
+      <c r="J46" s="25"/>
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
@@ -35825,21 +36938,30 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
       <c r="S46" s="24"/>
-      <c r="T46" s="26"/>
+      <c r="T46" s="24"/>
+      <c r="U46" s="24"/>
+      <c r="V46" s="24"/>
+      <c r="W46" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D45">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>D5=MIN($D$5:$D$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G45">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>G5=MIN($G$5:$G$45)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J45">
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>J5=MIN($J$5:$J$45)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36586,7 +37708,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36599,8 +37721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA71031-310C-CA40-B254-04EF996DC8FC}">
   <dimension ref="B1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36641,7 +37763,12 @@
       <c r="W2" s="17">
         <v>1.6856271298350999E-2</v>
       </c>
-      <c r="Z2" s="17"/>
+      <c r="Y2">
+        <v>175</v>
+      </c>
+      <c r="Z2">
+        <v>1.26891028702356E-2</v>
+      </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
@@ -36673,7 +37800,12 @@
       <c r="W3" s="17">
         <v>2.1516611400833999E-2</v>
       </c>
-      <c r="Z3" s="17"/>
+      <c r="Y3">
+        <v>176</v>
+      </c>
+      <c r="Z3">
+        <v>1.3078497769001E-2</v>
+      </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B4" s="21"/>
@@ -36709,7 +37841,12 @@
       <c r="W4" s="17">
         <v>1.31332652467962E-2</v>
       </c>
-      <c r="Z4" s="17"/>
+      <c r="Y4">
+        <v>177</v>
+      </c>
+      <c r="Z4">
+        <v>1.7109871524028399E-2</v>
+      </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
@@ -36720,8 +37857,12 @@
         <v>1.6856271298350999E-2</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
+      <c r="F5" s="11">
+        <v>175</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1.26891028702356E-2</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -36741,7 +37882,12 @@
       <c r="W5" s="17">
         <v>1.6341107195783602E-2</v>
       </c>
-      <c r="Z5" s="17"/>
+      <c r="Y5">
+        <v>178</v>
+      </c>
+      <c r="Z5">
+        <v>1.02781232201149E-2</v>
+      </c>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" s="21"/>
@@ -36752,8 +37898,12 @@
         <v>2.1516611400833999E-2</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="F6" s="11">
+        <v>176</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1.3078497769001E-2</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -36773,6 +37923,12 @@
       <c r="W6">
         <v>1.79924172089642E-2</v>
       </c>
+      <c r="Y6">
+        <v>179</v>
+      </c>
+      <c r="Z6">
+        <v>1.6296509506035201E-2</v>
+      </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
@@ -36783,8 +37939,12 @@
         <v>1.31332652467962E-2</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="F7" s="11">
+        <v>177</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1.7109871524028399E-2</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -36804,6 +37964,12 @@
       <c r="W7">
         <v>1.26500793800364E-2</v>
       </c>
+      <c r="Y7">
+        <v>180</v>
+      </c>
+      <c r="Z7">
+        <v>1.6147161229583401E-2</v>
+      </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="21"/>
@@ -36814,8 +37980,12 @@
         <v>1.6341107195783602E-2</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="11">
+        <v>178</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1.02781232201149E-2</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -36835,6 +38005,12 @@
       <c r="W8">
         <v>1.82553450711847E-2</v>
       </c>
+      <c r="Y8">
+        <v>181</v>
+      </c>
+      <c r="Z8">
+        <v>1.5810015095619901E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="21"/>
@@ -36845,8 +38021,12 @@
         <v>1.79924172089642E-2</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="F9" s="11">
+        <v>179</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1.6296509506035201E-2</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -36866,6 +38046,12 @@
       <c r="W9">
         <v>1.51738105473238E-2</v>
       </c>
+      <c r="Y9">
+        <v>182</v>
+      </c>
+      <c r="Z9">
+        <v>1.15689949576817E-2</v>
+      </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10" s="21"/>
@@ -36876,8 +38062,12 @@
         <v>1.26500793800364E-2</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="F10" s="11">
+        <v>180</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1.6147161229583401E-2</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -36897,6 +38087,12 @@
       <c r="W10">
         <v>1.8263229350767698E-2</v>
       </c>
+      <c r="Y10">
+        <v>183</v>
+      </c>
+      <c r="Z10">
+        <v>1.5105817138248099E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="21"/>
@@ -36907,8 +38103,12 @@
         <v>1.82553450711847E-2</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="F11" s="11">
+        <v>181</v>
+      </c>
+      <c r="G11" s="12">
+        <v>1.5810015095619901E-2</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -36928,6 +38128,12 @@
       <c r="W11">
         <v>1.7964500078156101E-2</v>
       </c>
+      <c r="Y11">
+        <v>184</v>
+      </c>
+      <c r="Z11">
+        <v>1.5156246825163699E-2</v>
+      </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="21"/>
@@ -36938,8 +38144,12 @@
         <v>1.51738105473238E-2</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
+      <c r="F12" s="11">
+        <v>182</v>
+      </c>
+      <c r="G12" s="12">
+        <v>1.15689949576817E-2</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -36959,6 +38169,12 @@
       <c r="W12">
         <v>1.0155658577741601E-2</v>
       </c>
+      <c r="Y12">
+        <v>185</v>
+      </c>
+      <c r="Z12">
+        <v>1.7064412699316699E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="21"/>
@@ -36969,8 +38185,12 @@
         <v>1.8263229350767698E-2</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
+      <c r="F13" s="11">
+        <v>183</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1.5105817138248099E-2</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -36990,6 +38210,12 @@
       <c r="W13">
         <v>1.26020955860629E-2</v>
       </c>
+      <c r="Y13">
+        <v>186</v>
+      </c>
+      <c r="Z13">
+        <v>1.84174780785996E-2</v>
+      </c>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B14" s="21"/>
@@ -37000,8 +38226,12 @@
         <v>1.7964500078156101E-2</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="11">
+        <v>184</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1.5156246825163699E-2</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -37021,6 +38251,12 @@
       <c r="W14">
         <v>1.3794482292036401E-2</v>
       </c>
+      <c r="Y14">
+        <v>187</v>
+      </c>
+      <c r="Z14">
+        <v>1.07580128328108E-2</v>
+      </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="21"/>
@@ -37031,8 +38267,12 @@
         <v>1.0155658577741601E-2</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
+      <c r="F15" s="11">
+        <v>185</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1.7064412699316699E-2</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -37052,6 +38292,12 @@
       <c r="W15">
         <v>1.7739876866237299E-2</v>
       </c>
+      <c r="Y15">
+        <v>188</v>
+      </c>
+      <c r="Z15">
+        <v>1.5512527721222601E-2</v>
+      </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="21"/>
@@ -37062,8 +38308,12 @@
         <v>1.26020955860629E-2</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
+      <c r="F16" s="11">
+        <v>186</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1.84174780785996E-2</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -37083,8 +38333,14 @@
       <c r="W16">
         <v>1.27215484780187E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y16">
+        <v>189</v>
+      </c>
+      <c r="Z16">
+        <v>1.8422442362240901E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B17" s="21"/>
       <c r="C17" s="11">
         <v>187</v>
@@ -37093,8 +38349,12 @@
         <v>1.3794482292036401E-2</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
+      <c r="F17" s="11">
+        <v>187</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1.07580128328108E-2</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -37114,8 +38374,14 @@
       <c r="W17">
         <v>1.6006272641558201E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y17">
+        <v>190</v>
+      </c>
+      <c r="Z17">
+        <v>1.6168670944827001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B18" s="21"/>
       <c r="C18" s="11">
         <v>188</v>
@@ -37124,8 +38390,12 @@
         <v>1.7739876866237299E-2</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
+      <c r="F18" s="11">
+        <v>188</v>
+      </c>
+      <c r="G18" s="12">
+        <v>1.5512527721222601E-2</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -37145,8 +38415,14 @@
       <c r="W18">
         <v>1.44282728094169E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y18">
+        <v>191</v>
+      </c>
+      <c r="Z18">
+        <v>1.3789475995308E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B19" s="21"/>
       <c r="C19" s="11">
         <v>189</v>
@@ -37155,8 +38431,12 @@
         <v>1.27215484780187E-2</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
+      <c r="F19" s="11">
+        <v>189</v>
+      </c>
+      <c r="G19" s="12">
+        <v>1.8422442362240901E-2</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -37176,8 +38456,14 @@
       <c r="W19">
         <v>1.2459204461490301E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y19">
+        <v>192</v>
+      </c>
+      <c r="Z19">
+        <v>1.26480493476688E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B20" s="21"/>
       <c r="C20" s="11">
         <v>190</v>
@@ -37186,8 +38472,12 @@
         <v>1.6006272641558201E-2</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="12"/>
+      <c r="F20" s="11">
+        <v>190</v>
+      </c>
+      <c r="G20" s="12">
+        <v>1.6168670944827001E-2</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -37207,8 +38497,14 @@
       <c r="W20">
         <v>1.74275668471052E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y20">
+        <v>193</v>
+      </c>
+      <c r="Z20">
+        <v>1.6373147451466299E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B21" s="21"/>
       <c r="C21" s="11">
         <v>191</v>
@@ -37217,8 +38513,12 @@
         <v>1.44282728094169E-2</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
+      <c r="F21" s="11">
+        <v>191</v>
+      </c>
+      <c r="G21" s="12">
+        <v>1.3789475995308E-2</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -37238,8 +38538,14 @@
       <c r="W21">
         <v>1.30827160444863E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y21">
+        <v>194</v>
+      </c>
+      <c r="Z21">
+        <v>1.77575115834975E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B22" s="21"/>
       <c r="C22" s="11">
         <v>192</v>
@@ -37248,8 +38554,12 @@
         <v>1.2459204461490301E-2</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="12"/>
+      <c r="F22" s="11">
+        <v>192</v>
+      </c>
+      <c r="G22" s="12">
+        <v>1.26480493476688E-2</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -37269,8 +38579,14 @@
       <c r="W22">
         <v>1.2280650395478E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="Y22">
+        <v>195</v>
+      </c>
+      <c r="Z22">
+        <v>1.5809258624735999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B23" s="21"/>
       <c r="C23" s="11">
         <v>193</v>
@@ -37279,8 +38595,12 @@
         <v>1.74275668471052E-2</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
+      <c r="F23" s="11">
+        <v>193</v>
+      </c>
+      <c r="G23" s="12">
+        <v>1.6373147451466299E-2</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -37295,7 +38615,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="22"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B24" s="21"/>
       <c r="C24" s="11">
         <v>194</v>
@@ -37304,8 +38624,12 @@
         <v>1.30827160444863E-2</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="11">
+        <v>194</v>
+      </c>
+      <c r="G24" s="12">
+        <v>1.77575115834975E-2</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -37320,7 +38644,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="22"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B25" s="21"/>
       <c r="C25" s="13">
         <v>195</v>
@@ -37329,8 +38653,12 @@
         <v>1.2280650395478E-2</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="13">
+        <v>195</v>
+      </c>
+      <c r="G25" s="14">
+        <v>1.5809258624735999E-2</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -37345,7 +38673,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="22"/>
     </row>
-    <row r="26" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
@@ -37372,12 +38700,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D25">
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="12" priority="20">
       <formula>D5=MIN($D$5:$D$25)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G25">
-    <cfRule type="expression" dxfId="0" priority="22">
+    <cfRule type="expression" dxfId="11" priority="22">
       <formula>G5=MIN($G$5:$G$25)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39182,42 +40510,42 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D40:D68">
-    <cfRule type="expression" dxfId="34" priority="16">
+    <cfRule type="expression" dxfId="43" priority="16">
       <formula>D40=MIN($D$40:$D$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:G68">
-    <cfRule type="expression" dxfId="33" priority="15">
+    <cfRule type="expression" dxfId="42" priority="15">
       <formula>G40=MIN($G$40:$G$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72:D87">
-    <cfRule type="expression" dxfId="32" priority="8">
+    <cfRule type="expression" dxfId="41" priority="8">
       <formula>D72=MIN($D$40:$D$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G72:G88">
-    <cfRule type="expression" dxfId="31" priority="6">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>G72=MIN($G$40:$G$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88">
-    <cfRule type="expression" dxfId="30" priority="5">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>D88=MIN($G$40:$G$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D89">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="38" priority="4">
       <formula>D89=MIN($G$40:$G$68)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="28" priority="3">
+    <cfRule type="expression" dxfId="37" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="36" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39965,7 +41293,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41392,12 +42720,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="34" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="24" priority="1">
+    <cfRule type="expression" dxfId="33" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42273,12 +43601,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="23" priority="3">
+    <cfRule type="expression" dxfId="32" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="22" priority="1">
+    <cfRule type="expression" dxfId="31" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43026,7 +44354,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="30" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43934,12 +45262,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="29" priority="3">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G33">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="28" priority="1">
       <formula>G5=MIN($G$5:$G$33)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45588,12 +46916,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D41">
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="27" priority="6">
       <formula>D5=MIN($D$5:$D$41)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G41">
-    <cfRule type="expression" dxfId="17" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>G5=MIN($G$5:$G$41)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46341,7 +47669,7 @@
     <mergeCell ref="C3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:D33">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>D5=MIN($D$5:$D$33)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>